<commit_message>
FIX test case 4
</commit_message>
<xml_diff>
--- a/GATEWAY/A1#111PROACTIVEXX/Proactive/Labpro/5.0/report-checklist.xlsx
+++ b/GATEWAY/A1#111PROACTIVEXX/Proactive/Labpro/5.0/report-checklist.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\vb_net_prj\API_REGIONETOSCANA\FSE 2.0\perValidazione\TESTCASEVALIDI\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{9BD3140D-D980-439D-B2AC-5B580210BA4D}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{81325940-578E-48A7-AE65-C8E5E1FB251B}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" activeTab="2" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -65,7 +65,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="352" uniqueCount="186">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="352" uniqueCount="185">
   <si>
     <t>COME VALORIZZARE LA CHECKLIST (tab TestCases)</t>
   </si>
@@ -755,22 +755,10 @@
     <t>20240102171337</t>
   </si>
   <si>
-    <t>2.16.840.1.113883.2.9.2.120.4.4.97bb3fc5bee3032679f4f07419e04af6375baafa17024527a98ede920c6812ed.1c527ef88b^^^^urn:ihe:iti:xdw:2013:workflowInstanceId</t>
-  </si>
-  <si>
-    <t>cee865c7a119ad5c</t>
-  </si>
-  <si>
-    <t>20240103122838</t>
-  </si>
-  <si>
     <t>2.16.840.1.113883.2.9.2.120.4.4.97bb3fc5bee3032679f4f07419e04af6375baafa17024527a98ede920c6812ed.60f361d4f3^^^^urn:ihe:iti:xdw:2013:workflowInstanceId</t>
   </si>
   <si>
     <t>ae18c270c07de1c9</t>
-  </si>
-  <si>
-    <t>20240103153951</t>
   </si>
   <si>
     <t>UNKNOWN_WORKFLOW_ID</t>
@@ -835,6 +823,15 @@
   </si>
   <si>
     <t>20240110133242</t>
+  </si>
+  <si>
+    <t>20240111095628</t>
+  </si>
+  <si>
+    <t>27739902048d99eb</t>
+  </si>
+  <si>
+    <t>2.16.840.1.113883.2.9.2.120.4.4.97bb3fc5bee3032679f4f07419e04af6375baafa17024527a98ede920c6812ed.63f805c6a2^^^^urn:ihe:iti:xdw:2013:workflowInstanceId</t>
   </si>
 </sst>
 </file>
@@ -1769,10 +1766,10 @@
   <dimension ref="A1:T644"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="70" zoomScaleNormal="70" workbookViewId="0">
-      <pane xSplit="1" ySplit="9" topLeftCell="E10" activePane="bottomRight" state="frozen"/>
+      <pane xSplit="1" ySplit="9" topLeftCell="B10" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight" activeCell="B1" sqref="B1"/>
       <selection pane="bottomLeft" activeCell="A10" sqref="A10"/>
-      <selection pane="bottomRight" activeCell="F16" sqref="F16"/>
+      <selection pane="bottomRight" activeCell="G13" sqref="G13"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="14.42578125" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -2175,16 +2172,16 @@
         <v>54</v>
       </c>
       <c r="F13" s="23">
-        <v>45294</v>
+        <v>45302</v>
       </c>
       <c r="G13" s="33" t="s">
-        <v>161</v>
+        <v>182</v>
       </c>
       <c r="H13" s="24" t="s">
-        <v>160</v>
+        <v>183</v>
       </c>
       <c r="I13" s="24" t="s">
-        <v>159</v>
+        <v>184</v>
       </c>
       <c r="J13" s="25" t="s">
         <v>71</v>
@@ -2222,13 +2219,13 @@
         <v>45294</v>
       </c>
       <c r="G14" s="33" t="s">
-        <v>164</v>
+        <v>182</v>
       </c>
       <c r="H14" s="24" t="s">
-        <v>163</v>
+        <v>160</v>
       </c>
       <c r="I14" s="24" t="s">
-        <v>162</v>
+        <v>159</v>
       </c>
       <c r="J14" s="25" t="s">
         <v>71</v>
@@ -2266,13 +2263,13 @@
         <v>45301</v>
       </c>
       <c r="G15" s="33" t="s">
-        <v>183</v>
+        <v>179</v>
       </c>
       <c r="H15" s="24" t="s">
-        <v>182</v>
+        <v>178</v>
       </c>
       <c r="I15" s="24" t="s">
-        <v>165</v>
+        <v>161</v>
       </c>
       <c r="J15" s="25" t="s">
         <v>71</v>
@@ -2285,13 +2282,13 @@
         <v>71</v>
       </c>
       <c r="N15" s="25" t="s">
-        <v>166</v>
+        <v>162</v>
       </c>
       <c r="O15" s="25" t="s">
         <v>71</v>
       </c>
       <c r="P15" s="25" t="s">
-        <v>181</v>
+        <v>177</v>
       </c>
       <c r="Q15" s="25"/>
       <c r="R15" s="26"/>
@@ -2320,13 +2317,13 @@
         <v>45301</v>
       </c>
       <c r="G16" s="33" t="s">
-        <v>185</v>
+        <v>181</v>
       </c>
       <c r="H16" s="24" t="s">
-        <v>184</v>
+        <v>180</v>
       </c>
       <c r="I16" s="24" t="s">
-        <v>165</v>
+        <v>161</v>
       </c>
       <c r="J16" s="25" t="s">
         <v>71</v>
@@ -2339,13 +2336,13 @@
         <v>71</v>
       </c>
       <c r="N16" s="25" t="s">
-        <v>167</v>
+        <v>163</v>
       </c>
       <c r="O16" s="25" t="s">
         <v>71</v>
       </c>
       <c r="P16" s="25" t="s">
-        <v>181</v>
+        <v>177</v>
       </c>
       <c r="Q16" s="25"/>
       <c r="R16" s="26"/>
@@ -2383,13 +2380,13 @@
         <v>71</v>
       </c>
       <c r="N17" s="25" t="s">
-        <v>169</v>
+        <v>165</v>
       </c>
       <c r="O17" s="25" t="s">
         <v>71</v>
       </c>
       <c r="P17" s="25" t="s">
-        <v>168</v>
+        <v>164</v>
       </c>
       <c r="Q17" s="25"/>
       <c r="R17" s="26"/>
@@ -2422,7 +2419,7 @@
         <v>145</v>
       </c>
       <c r="K18" s="25" t="s">
-        <v>170</v>
+        <v>166</v>
       </c>
       <c r="L18" s="25"/>
       <c r="M18" s="25"/>
@@ -2460,14 +2457,14 @@
         <v>145</v>
       </c>
       <c r="K19" s="25" t="s">
-        <v>180</v>
+        <v>176</v>
       </c>
       <c r="L19" s="25"/>
       <c r="M19" s="25"/>
       <c r="N19" s="25"/>
       <c r="O19" s="25"/>
       <c r="P19" s="25" t="s">
-        <v>171</v>
+        <v>167</v>
       </c>
       <c r="Q19" s="25"/>
       <c r="R19" s="26"/>
@@ -2500,7 +2497,7 @@
         <v>145</v>
       </c>
       <c r="K20" s="25" t="s">
-        <v>172</v>
+        <v>168</v>
       </c>
       <c r="L20" s="25"/>
       <c r="M20" s="25"/>
@@ -2538,7 +2535,7 @@
         <v>145</v>
       </c>
       <c r="K21" s="25" t="s">
-        <v>179</v>
+        <v>175</v>
       </c>
       <c r="L21" s="25"/>
       <c r="M21" s="25"/>
@@ -2576,7 +2573,7 @@
         <v>145</v>
       </c>
       <c r="K22" s="25" t="s">
-        <v>173</v>
+        <v>169</v>
       </c>
       <c r="L22" s="25"/>
       <c r="M22" s="25"/>
@@ -2614,7 +2611,7 @@
         <v>145</v>
       </c>
       <c r="K23" s="25" t="s">
-        <v>174</v>
+        <v>170</v>
       </c>
       <c r="L23" s="25"/>
       <c r="M23" s="25"/>
@@ -2652,7 +2649,7 @@
         <v>145</v>
       </c>
       <c r="K24" s="25" t="s">
-        <v>175</v>
+        <v>171</v>
       </c>
       <c r="L24" s="25"/>
       <c r="M24" s="25"/>
@@ -2690,7 +2687,7 @@
         <v>145</v>
       </c>
       <c r="K25" s="25" t="s">
-        <v>176</v>
+        <v>172</v>
       </c>
       <c r="L25" s="25"/>
       <c r="M25" s="25"/>
@@ -2728,7 +2725,7 @@
         <v>145</v>
       </c>
       <c r="K26" s="25" t="s">
-        <v>177</v>
+        <v>173</v>
       </c>
       <c r="L26" s="25"/>
       <c r="M26" s="25"/>
@@ -2766,7 +2763,7 @@
         <v>145</v>
       </c>
       <c r="K27" s="25" t="s">
-        <v>178</v>
+        <v>174</v>
       </c>
       <c r="L27" s="25"/>
       <c r="M27" s="25"/>

</xml_diff>

<commit_message>
Aggiunto ID 62 - Test Case KO 16
</commit_message>
<xml_diff>
--- a/GATEWAY/A1#111PROACTIVEXX/Proactive/Labpro/5.0/report-checklist.xlsx
+++ b/GATEWAY/A1#111PROACTIVEXX/Proactive/Labpro/5.0/report-checklist.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\vb_net_prj\API_REGIONETOSCANA\FSE 2.0\perValidazione\TESTCASEVALIDI\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{81325940-578E-48A7-AE65-C8E5E1FB251B}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{21C5BEA1-BEAA-400D-AC97-C3B43656672F}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" activeTab="2" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -65,7 +65,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="352" uniqueCount="185">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="366" uniqueCount="191">
   <si>
     <t>COME VALORIZZARE LA CHECKLIST (tab TestCases)</t>
   </si>
@@ -833,6 +833,25 @@
   <si>
     <t>2.16.840.1.113883.2.9.2.120.4.4.97bb3fc5bee3032679f4f07419e04af6375baafa17024527a98ede920c6812ed.63f805c6a2^^^^urn:ihe:iti:xdw:2013:workflowInstanceId</t>
   </si>
+  <si>
+    <t>VALIDAZIONE_CDA2_LAB_CT16_KO</t>
+  </si>
+  <si>
+    <t>Viene richiamato il servizio di validazione "https://&lt;HOST&gt;:&lt;PORT&gt;/v&lt;major&gt;/documents/validation"al fine di testare la gestione degli errori semantici sui Dati (status code 422), secondo quanto descritto in https://github.com/ministero-salute/it-fse-support/tree/main/doc/integrazione-gateway.
+I dati utilizzati per comporre il CDA2 dovranno essere conformi alle section e le entry secondo quanto nella sezione "CASO DI TEST 16" riportata nei documenti "casi di test LAB" e "CDA2_Referto Medicina di Laboratorio_KO" presenti al path https://github.com/ministero-salute/it-fse-accreditamento.</t>
+  </si>
+  <si>
+    <t>20240112180353</t>
+  </si>
+  <si>
+    <t>38307b48881219da</t>
+  </si>
+  <si>
+    <t>2.16.840.1.113883.2.9.2.120.4.4.97bb3fc5bee3032679f4f07419e04af6375baafa17024527a98ede920c6812ed.dff24801c3^^^^urn:ihe:iti:xdw:2013:workflowInstanceId</t>
+  </si>
+  <si>
+    <t>[W002 | Si consiglia di valorizzare l'elemento organizer[CLUSTER]/code]</t>
+  </si>
 </sst>
 </file>
 
@@ -841,7 +860,7 @@
   <numFmts count="1">
     <numFmt numFmtId="164" formatCode="d/m/yyyy"/>
   </numFmts>
-  <fonts count="9" x14ac:knownFonts="1">
+  <fonts count="10" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -900,6 +919,11 @@
       <color theme="1"/>
       <name val="Calibri"/>
       <family val="2"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color theme="1"/>
+      <name val="Calibri"/>
     </font>
   </fonts>
   <fills count="4">
@@ -1162,7 +1186,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="46">
+  <cellXfs count="56">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
@@ -1253,6 +1277,36 @@
       <alignment horizontal="right" wrapText="1"/>
     </xf>
     <xf numFmtId="164" fontId="2" fillId="0" borderId="17" xfId="0" quotePrefix="1" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1" readingOrder="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="0" borderId="17" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="164" fontId="9" fillId="0" borderId="3" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1" readingOrder="1"/>
+    </xf>
+    <xf numFmtId="164" fontId="9" fillId="0" borderId="17" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1" readingOrder="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="0" borderId="17" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="49" fontId="9" fillId="0" borderId="17" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="0" borderId="18" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="0" borderId="18" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="164" fontId="9" fillId="0" borderId="17" xfId="0" quotePrefix="1" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1" readingOrder="1"/>
     </xf>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
@@ -1766,10 +1820,10 @@
   <dimension ref="A1:T644"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="70" zoomScaleNormal="70" workbookViewId="0">
-      <pane xSplit="1" ySplit="9" topLeftCell="B10" activePane="bottomRight" state="frozen"/>
+      <pane xSplit="1" ySplit="9" topLeftCell="B26" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight" activeCell="B1" sqref="B1"/>
       <selection pane="bottomLeft" activeCell="A10" sqref="A10"/>
-      <selection pane="bottomRight" activeCell="G13" sqref="G13"/>
+      <selection pane="bottomRight" activeCell="E28" sqref="E28"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="14.42578125" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1808,14 +1862,14 @@
       <c r="T1" s="15"/>
     </row>
     <row r="2" spans="1:20" ht="18.75" x14ac:dyDescent="0.25">
-      <c r="A2" s="36" t="s">
+      <c r="A2" s="46" t="s">
         <v>22</v>
       </c>
-      <c r="B2" s="37"/>
-      <c r="C2" s="38" t="s">
+      <c r="B2" s="47"/>
+      <c r="C2" s="48" t="s">
         <v>146</v>
       </c>
-      <c r="D2" s="37"/>
+      <c r="D2" s="47"/>
       <c r="F2" s="12"/>
       <c r="G2" s="12"/>
       <c r="H2" s="12"/>
@@ -1833,14 +1887,14 @@
       <c r="T2" s="15"/>
     </row>
     <row r="3" spans="1:20" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="A3" s="39" t="s">
+      <c r="A3" s="49" t="s">
         <v>23</v>
       </c>
-      <c r="B3" s="40"/>
-      <c r="C3" s="45" t="s">
+      <c r="B3" s="50"/>
+      <c r="C3" s="55" t="s">
         <v>149</v>
       </c>
-      <c r="D3" s="37"/>
+      <c r="D3" s="47"/>
       <c r="F3" s="12"/>
       <c r="G3" s="12"/>
       <c r="H3" s="12"/>
@@ -1858,12 +1912,12 @@
       <c r="T3" s="15"/>
     </row>
     <row r="4" spans="1:20" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="A4" s="41"/>
-      <c r="B4" s="42"/>
-      <c r="C4" s="45" t="s">
+      <c r="A4" s="51"/>
+      <c r="B4" s="52"/>
+      <c r="C4" s="55" t="s">
         <v>148</v>
       </c>
-      <c r="D4" s="37"/>
+      <c r="D4" s="47"/>
       <c r="E4" s="4"/>
       <c r="F4" s="12"/>
       <c r="G4" s="12"/>
@@ -1882,12 +1936,12 @@
       <c r="T4" s="15"/>
     </row>
     <row r="5" spans="1:20" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="A5" s="43"/>
-      <c r="B5" s="44"/>
-      <c r="C5" s="45" t="s">
+      <c r="A5" s="53"/>
+      <c r="B5" s="54"/>
+      <c r="C5" s="55" t="s">
         <v>147</v>
       </c>
-      <c r="D5" s="37"/>
+      <c r="D5" s="47"/>
       <c r="F5" s="12"/>
       <c r="G5" s="12"/>
       <c r="H5" s="12"/>
@@ -1905,8 +1959,8 @@
       <c r="T5" s="15"/>
     </row>
     <row r="6" spans="1:20" x14ac:dyDescent="0.25">
-      <c r="A6" s="34"/>
-      <c r="B6" s="35"/>
+      <c r="A6" s="44"/>
+      <c r="B6" s="45"/>
       <c r="C6" s="16"/>
       <c r="F6" s="12"/>
       <c r="G6" s="12"/>
@@ -2739,7 +2793,7 @@
         <v>64</v>
       </c>
     </row>
-    <row r="27" spans="1:20" ht="36" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="27" spans="1:20" ht="36" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A27" s="20">
         <v>61</v>
       </c>
@@ -2777,22 +2831,59 @@
         <v>64</v>
       </c>
     </row>
-    <row r="28" spans="1:20" x14ac:dyDescent="0.25">
-      <c r="F28" s="12"/>
-      <c r="G28" s="12"/>
-      <c r="H28" s="12"/>
-      <c r="I28" s="12"/>
-      <c r="J28" s="13"/>
-      <c r="K28" s="13"/>
-      <c r="L28" s="13"/>
-      <c r="M28" s="13"/>
-      <c r="N28" s="13"/>
-      <c r="O28" s="13"/>
-      <c r="P28" s="13"/>
-      <c r="Q28" s="13"/>
-      <c r="R28" s="14"/>
-      <c r="S28" s="2"/>
-      <c r="T28" s="15"/>
+    <row r="28" spans="1:20" ht="180" x14ac:dyDescent="0.25">
+      <c r="A28" s="34">
+        <v>62</v>
+      </c>
+      <c r="B28" s="35" t="s">
+        <v>44</v>
+      </c>
+      <c r="C28" s="35" t="s">
+        <v>45</v>
+      </c>
+      <c r="D28" s="35" t="s">
+        <v>185</v>
+      </c>
+      <c r="E28" s="36" t="s">
+        <v>186</v>
+      </c>
+      <c r="F28" s="37">
+        <v>45303</v>
+      </c>
+      <c r="G28" s="43" t="s">
+        <v>187</v>
+      </c>
+      <c r="H28" s="38" t="s">
+        <v>188</v>
+      </c>
+      <c r="I28" s="38" t="s">
+        <v>189</v>
+      </c>
+      <c r="J28" s="25" t="s">
+        <v>71</v>
+      </c>
+      <c r="K28" s="39"/>
+      <c r="L28" s="25" t="s">
+        <v>71</v>
+      </c>
+      <c r="M28" s="25" t="s">
+        <v>71</v>
+      </c>
+      <c r="N28" s="39" t="s">
+        <v>190</v>
+      </c>
+      <c r="O28" s="25" t="s">
+        <v>71</v>
+      </c>
+      <c r="P28" s="25" t="s">
+        <v>177</v>
+      </c>
+      <c r="Q28" s="39"/>
+      <c r="R28" s="40"/>
+      <c r="S28" s="41"/>
+      <c r="T28" s="42" t="s">
+        <v>64</v>
+      </c>
     </row>
     <row r="29" spans="1:20" x14ac:dyDescent="0.25">
       <c r="F29" s="12"/>
@@ -7449,7 +7540,7 @@
           <x14:formula1>
             <xm:f>Sheet1!$B$2:$B$3</xm:f>
           </x14:formula1>
-          <xm:sqref>O10:O27 L10:M27 J10:J27</xm:sqref>
+          <xm:sqref>O10:O28 J10:J28 L10:M28</xm:sqref>
         </x14:dataValidation>
         <x14:dataValidation type="list" allowBlank="1" showErrorMessage="1" xr:uid="{00000000-0002-0000-0200-000001000000}">
           <x14:formula1>
@@ -7470,7 +7561,7 @@
   <sheetViews>
     <sheetView workbookViewId="0">
       <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="D2" sqref="D2"/>
+      <selection pane="bottomLeft" activeCell="B1014" sqref="B1014"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="14.42578125" defaultRowHeight="15" customHeight="1" x14ac:dyDescent="0.25"/>

</xml_diff>

<commit_message>
Ricaricati TEST CASE KO 28,36
</commit_message>
<xml_diff>
--- a/GATEWAY/A1#111PROACTIVEXX/Proactive/Labpro/5.0/report-checklist.xlsx
+++ b/GATEWAY/A1#111PROACTIVEXX/Proactive/Labpro/5.0/report-checklist.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\vb_net_prj\API_REGIONETOSCANA\FSE 2.0\perValidazione\TESTCASEVALIDI\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{21C5BEA1-BEAA-400D-AC97-C3B43656672F}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{0752CB78-829F-4FDD-8247-D4B8BD8117DE}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" activeTab="2" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -813,18 +813,6 @@
     <t>L'utente riceve una segnalazione che indica di aprire un ticket verso Proactive e uno dei Nostri addetti risolverà il proplema in assistenza remota</t>
   </si>
   <si>
-    <t>0ed9c44f781b1f31</t>
-  </si>
-  <si>
-    <t>20240110132717</t>
-  </si>
-  <si>
-    <t>23102b9be18ec2b9</t>
-  </si>
-  <si>
-    <t>20240110133242</t>
-  </si>
-  <si>
     <t>20240111095628</t>
   </si>
   <si>
@@ -851,6 +839,18 @@
   </si>
   <si>
     <t>[W002 | Si consiglia di valorizzare l'elemento organizer[CLUSTER]/code]</t>
+  </si>
+  <si>
+    <t>20240115173748</t>
+  </si>
+  <si>
+    <t>4ebe00312176e199</t>
+  </si>
+  <si>
+    <t>20240115174324</t>
+  </si>
+  <si>
+    <t>92038db3af751528</t>
   </si>
 </sst>
 </file>
@@ -1820,10 +1820,10 @@
   <dimension ref="A1:T644"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="70" zoomScaleNormal="70" workbookViewId="0">
-      <pane xSplit="1" ySplit="9" topLeftCell="B26" activePane="bottomRight" state="frozen"/>
+      <pane xSplit="1" ySplit="9" topLeftCell="E10" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight" activeCell="B1" sqref="B1"/>
       <selection pane="bottomLeft" activeCell="A10" sqref="A10"/>
-      <selection pane="bottomRight" activeCell="E28" sqref="E28"/>
+      <selection pane="bottomRight" activeCell="G15" sqref="G15"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="14.42578125" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -2229,13 +2229,13 @@
         <v>45302</v>
       </c>
       <c r="G13" s="33" t="s">
-        <v>182</v>
+        <v>178</v>
       </c>
       <c r="H13" s="24" t="s">
-        <v>183</v>
+        <v>179</v>
       </c>
       <c r="I13" s="24" t="s">
-        <v>184</v>
+        <v>180</v>
       </c>
       <c r="J13" s="25" t="s">
         <v>71</v>
@@ -2253,7 +2253,7 @@
         <v>48</v>
       </c>
     </row>
-    <row r="14" spans="1:20" ht="36" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="14" spans="1:20" ht="36" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A14" s="20">
         <v>5</v>
       </c>
@@ -2273,7 +2273,7 @@
         <v>45294</v>
       </c>
       <c r="G14" s="33" t="s">
-        <v>182</v>
+        <v>178</v>
       </c>
       <c r="H14" s="24" t="s">
         <v>160</v>
@@ -2297,7 +2297,7 @@
         <v>48</v>
       </c>
     </row>
-    <row r="15" spans="1:20" ht="36" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="15" spans="1:20" ht="36" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A15" s="20">
         <v>28</v>
       </c>
@@ -2314,13 +2314,13 @@
         <v>63</v>
       </c>
       <c r="F15" s="23">
-        <v>45301</v>
+        <v>45306</v>
       </c>
       <c r="G15" s="33" t="s">
-        <v>179</v>
+        <v>187</v>
       </c>
       <c r="H15" s="24" t="s">
-        <v>178</v>
+        <v>188</v>
       </c>
       <c r="I15" s="24" t="s">
         <v>161</v>
@@ -2351,7 +2351,7 @@
         <v>64</v>
       </c>
     </row>
-    <row r="16" spans="1:20" ht="36" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="16" spans="1:20" ht="36" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A16" s="20">
         <v>36</v>
       </c>
@@ -2368,13 +2368,13 @@
         <v>68</v>
       </c>
       <c r="F16" s="23">
-        <v>45301</v>
+        <v>45306</v>
       </c>
       <c r="G16" s="33" t="s">
-        <v>181</v>
-      </c>
-      <c r="H16" s="24" t="s">
-        <v>180</v>
+        <v>189</v>
+      </c>
+      <c r="H16" s="33" t="s">
+        <v>190</v>
       </c>
       <c r="I16" s="24" t="s">
         <v>161</v>
@@ -2405,7 +2405,7 @@
         <v>64</v>
       </c>
     </row>
-    <row r="17" spans="1:20" ht="36" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="17" spans="1:20" ht="36" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A17" s="20">
         <v>44</v>
       </c>
@@ -2842,22 +2842,22 @@
         <v>45</v>
       </c>
       <c r="D28" s="35" t="s">
-        <v>185</v>
+        <v>181</v>
       </c>
       <c r="E28" s="36" t="s">
-        <v>186</v>
+        <v>182</v>
       </c>
       <c r="F28" s="37">
         <v>45303</v>
       </c>
       <c r="G28" s="43" t="s">
-        <v>187</v>
+        <v>183</v>
       </c>
       <c r="H28" s="38" t="s">
-        <v>188</v>
+        <v>184</v>
       </c>
       <c r="I28" s="38" t="s">
-        <v>189</v>
+        <v>185</v>
       </c>
       <c r="J28" s="25" t="s">
         <v>71</v>
@@ -2870,7 +2870,7 @@
         <v>71</v>
       </c>
       <c r="N28" s="39" t="s">
-        <v>190</v>
+        <v>186</v>
       </c>
       <c r="O28" s="25" t="s">
         <v>71</v>

</xml_diff>

<commit_message>
Aggiunto test case 191
</commit_message>
<xml_diff>
--- a/GATEWAY/A1#111PROACTIVEXX/Proactive/Labpro/5.0/report-checklist.xlsx
+++ b/GATEWAY/A1#111PROACTIVEXX/Proactive/Labpro/5.0/report-checklist.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\vb_net_prj\API_REGIONETOSCANA\FSE 2.0\perValidazione\LAB+RAD+RSA\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{8F894B9A-2C68-4940-B583-3E6144A01B3F}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{23963DF1-F7B8-49FF-B3D5-6F224CB091E4}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" activeTab="2" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -65,7 +65,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="647" uniqueCount="292">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="656" uniqueCount="297">
   <si>
     <t>COME VALORIZZARE LA CHECKLIST (tab TestCases)</t>
   </si>
@@ -1253,6 +1253,24 @@
   </si>
   <si>
     <t xml:space="preserve"> il sesso del pazioente è gestito con trascodifica a livello applicativo nojn è possibile avere valori diversi da "male", "female" o "undifferentiated"</t>
+  </si>
+  <si>
+    <t>VALIDAZIONE_CDA2_LAB_TRASF_CT1</t>
+  </si>
+  <si>
+    <t xml:space="preserve">
+Viene richiamato il servizio di validazione "https://&lt;HOST&gt;:&lt;PORT&gt;/v&lt;major&gt;/documents/validation", al fine di una futura pubblicazione, con esito positivo (status code 201), secondo quanto descritto in https://github.com/ministero-salute/it-fse-support/tree/main/doc/integrazione-gateway.
+Il Documento CDA2 Laboratorio dovrà essere composto in moda da risultare valido dal punto di vista sintattico, semantico, terminologico. I dati utilizzati per comporre il CDA2 dovranno essere conformi alle section e le entry secondo quanto espresso dalla sezione "CASO DI TEST- OK" riportata nei documenti "Caso di test - Trasfusionale" e "CDA2_Trasfusionale_OK" presenti al path https://github.com/ministero-salute/it-fse-accreditamento.
+</t>
+  </si>
+  <si>
+    <t>20240122181755</t>
+  </si>
+  <si>
+    <t>6bc36adac097cf0b</t>
+  </si>
+  <si>
+    <t>2.16.840.1.113883.2.9.2.120.4.4.46a41df0ab0514f11c0811056832c3225e06c8e11824f27c7e5517ca5cfc57fe.d7a484329f^^^^urn:ihe:iti:xdw:2013:workflowInstanceId</t>
   </si>
 </sst>
 </file>
@@ -2273,10 +2291,10 @@
   <dimension ref="A1:T642"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="80" zoomScaleNormal="80" workbookViewId="0">
-      <pane xSplit="1" ySplit="9" topLeftCell="B10" activePane="bottomRight" state="frozen"/>
+      <pane xSplit="1" ySplit="9" topLeftCell="D10" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight" activeCell="B1" sqref="B1"/>
       <selection pane="bottomLeft" activeCell="A10" sqref="A10"/>
-      <selection pane="bottomRight" activeCell="A58" sqref="A58"/>
+      <selection pane="bottomRight" activeCell="G29" sqref="G29"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="14.42578125" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -3339,52 +3357,52 @@
       </c>
     </row>
     <row r="29" spans="1:20" s="46" customFormat="1" ht="20.100000000000001" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A29" s="45">
-        <v>11</v>
-      </c>
-      <c r="B29" s="26" t="s">
+      <c r="A29" s="35">
+        <v>191</v>
+      </c>
+      <c r="B29" s="36" t="s">
         <v>44</v>
       </c>
-      <c r="C29" s="26" t="s">
-        <v>57</v>
-      </c>
-      <c r="D29" s="26" t="s">
-        <v>144</v>
-      </c>
-      <c r="E29" s="27" t="s">
-        <v>145</v>
-      </c>
-      <c r="F29" s="28">
+      <c r="C29" s="36" t="s">
+        <v>45</v>
+      </c>
+      <c r="D29" s="36" t="s">
+        <v>292</v>
+      </c>
+      <c r="E29" s="37" t="s">
+        <v>293</v>
+      </c>
+      <c r="F29" s="38">
         <v>45313</v>
       </c>
-      <c r="G29" s="29" t="s">
-        <v>244</v>
-      </c>
-      <c r="H29" s="30" t="s">
-        <v>242</v>
-      </c>
-      <c r="I29" s="30" t="s">
-        <v>243</v>
-      </c>
-      <c r="J29" s="31" t="s">
+      <c r="G29" s="39" t="s">
+        <v>294</v>
+      </c>
+      <c r="H29" s="40" t="s">
+        <v>295</v>
+      </c>
+      <c r="I29" s="40" t="s">
+        <v>296</v>
+      </c>
+      <c r="J29" s="41" t="s">
         <v>66</v>
       </c>
-      <c r="K29" s="31"/>
-      <c r="L29" s="31"/>
-      <c r="M29" s="31"/>
-      <c r="N29" s="31"/>
-      <c r="O29" s="31"/>
-      <c r="P29" s="31"/>
-      <c r="Q29" s="31"/>
-      <c r="R29" s="32"/>
-      <c r="S29" s="33"/>
-      <c r="T29" s="34" t="s">
+      <c r="K29" s="41"/>
+      <c r="L29" s="41"/>
+      <c r="M29" s="41"/>
+      <c r="N29" s="41"/>
+      <c r="O29" s="41"/>
+      <c r="P29" s="41"/>
+      <c r="Q29" s="41"/>
+      <c r="R29" s="42"/>
+      <c r="S29" s="43"/>
+      <c r="T29" s="44" t="s">
         <v>48</v>
       </c>
     </row>
     <row r="30" spans="1:20" s="46" customFormat="1" ht="20.100000000000001" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A30" s="45">
-        <v>12</v>
+        <v>11</v>
       </c>
       <c r="B30" s="26" t="s">
         <v>44</v>
@@ -3393,21 +3411,27 @@
         <v>57</v>
       </c>
       <c r="D30" s="26" t="s">
-        <v>146</v>
+        <v>144</v>
       </c>
       <c r="E30" s="27" t="s">
-        <v>147</v>
-      </c>
-      <c r="F30" s="28"/>
-      <c r="G30" s="29"/>
-      <c r="H30" s="30"/>
-      <c r="I30" s="30"/>
+        <v>145</v>
+      </c>
+      <c r="F30" s="28">
+        <v>45313</v>
+      </c>
+      <c r="G30" s="29" t="s">
+        <v>244</v>
+      </c>
+      <c r="H30" s="30" t="s">
+        <v>242</v>
+      </c>
+      <c r="I30" s="30" t="s">
+        <v>243</v>
+      </c>
       <c r="J30" s="31" t="s">
-        <v>98</v>
-      </c>
-      <c r="K30" s="31" t="s">
-        <v>245</v>
-      </c>
+        <v>66</v>
+      </c>
+      <c r="K30" s="31"/>
       <c r="L30" s="31"/>
       <c r="M30" s="31"/>
       <c r="N30" s="31"/>
@@ -3422,7 +3446,7 @@
     </row>
     <row r="31" spans="1:20" s="46" customFormat="1" ht="20.100000000000001" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A31" s="45">
-        <v>13</v>
+        <v>12</v>
       </c>
       <c r="B31" s="26" t="s">
         <v>44</v>
@@ -3431,13 +3455,13 @@
         <v>57</v>
       </c>
       <c r="D31" s="26" t="s">
-        <v>148</v>
+        <v>146</v>
       </c>
       <c r="E31" s="27" t="s">
-        <v>149</v>
+        <v>147</v>
       </c>
       <c r="F31" s="28"/>
-      <c r="G31" s="30"/>
+      <c r="G31" s="29"/>
       <c r="H31" s="30"/>
       <c r="I31" s="30"/>
       <c r="J31" s="31" t="s">
@@ -3460,7 +3484,7 @@
     </row>
     <row r="32" spans="1:20" s="46" customFormat="1" ht="20.100000000000001" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A32" s="45">
-        <v>14</v>
+        <v>13</v>
       </c>
       <c r="B32" s="26" t="s">
         <v>44</v>
@@ -3469,10 +3493,10 @@
         <v>57</v>
       </c>
       <c r="D32" s="26" t="s">
-        <v>150</v>
+        <v>148</v>
       </c>
       <c r="E32" s="27" t="s">
-        <v>151</v>
+        <v>149</v>
       </c>
       <c r="F32" s="28"/>
       <c r="G32" s="30"/>
@@ -3497,8 +3521,8 @@
       </c>
     </row>
     <row r="33" spans="1:20" s="46" customFormat="1" ht="20.100000000000001" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A33" s="25">
-        <v>31</v>
+      <c r="A33" s="45">
+        <v>14</v>
       </c>
       <c r="B33" s="26" t="s">
         <v>44</v>
@@ -3507,52 +3531,36 @@
         <v>57</v>
       </c>
       <c r="D33" s="26" t="s">
-        <v>152</v>
+        <v>150</v>
       </c>
       <c r="E33" s="27" t="s">
-        <v>59</v>
-      </c>
-      <c r="F33" s="28">
-        <v>45313</v>
-      </c>
-      <c r="G33" s="29" t="s">
-        <v>246</v>
-      </c>
-      <c r="H33" s="30" t="s">
-        <v>247</v>
-      </c>
-      <c r="I33" s="30" t="s">
-        <v>114</v>
-      </c>
+        <v>151</v>
+      </c>
+      <c r="F33" s="28"/>
+      <c r="G33" s="30"/>
+      <c r="H33" s="30"/>
+      <c r="I33" s="30"/>
       <c r="J33" s="31" t="s">
-        <v>66</v>
-      </c>
-      <c r="K33" s="31"/>
-      <c r="L33" s="31" t="s">
         <v>98</v>
       </c>
-      <c r="M33" s="31" t="s">
-        <v>66</v>
-      </c>
-      <c r="N33" s="31" t="s">
-        <v>115</v>
-      </c>
-      <c r="O33" s="31" t="s">
-        <v>66</v>
-      </c>
-      <c r="P33" s="31" t="s">
-        <v>130</v>
-      </c>
+      <c r="K33" s="31" t="s">
+        <v>245</v>
+      </c>
+      <c r="L33" s="31"/>
+      <c r="M33" s="31"/>
+      <c r="N33" s="31"/>
+      <c r="O33" s="31"/>
+      <c r="P33" s="31"/>
       <c r="Q33" s="31"/>
       <c r="R33" s="32"/>
       <c r="S33" s="33"/>
       <c r="T33" s="34" t="s">
-        <v>60</v>
+        <v>48</v>
       </c>
     </row>
     <row r="34" spans="1:20" s="46" customFormat="1" ht="20.100000000000001" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A34" s="25">
-        <v>39</v>
+        <v>31</v>
       </c>
       <c r="B34" s="26" t="s">
         <v>44</v>
@@ -3561,19 +3569,19 @@
         <v>57</v>
       </c>
       <c r="D34" s="26" t="s">
-        <v>153</v>
+        <v>152</v>
       </c>
       <c r="E34" s="27" t="s">
-        <v>63</v>
+        <v>59</v>
       </c>
       <c r="F34" s="28">
         <v>45313</v>
       </c>
       <c r="G34" s="29" t="s">
-        <v>249</v>
+        <v>246</v>
       </c>
       <c r="H34" s="30" t="s">
-        <v>248</v>
+        <v>247</v>
       </c>
       <c r="I34" s="30" t="s">
         <v>114</v>
@@ -3589,7 +3597,7 @@
         <v>66</v>
       </c>
       <c r="N34" s="31" t="s">
-        <v>116</v>
+        <v>115</v>
       </c>
       <c r="O34" s="31" t="s">
         <v>66</v>
@@ -3606,7 +3614,7 @@
     </row>
     <row r="35" spans="1:20" s="46" customFormat="1" ht="20.100000000000001" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A35" s="25">
-        <v>47</v>
+        <v>39</v>
       </c>
       <c r="B35" s="26" t="s">
         <v>44</v>
@@ -3615,16 +3623,26 @@
         <v>57</v>
       </c>
       <c r="D35" s="26" t="s">
-        <v>154</v>
+        <v>153</v>
       </c>
       <c r="E35" s="27" t="s">
-        <v>65</v>
-      </c>
-      <c r="F35" s="28"/>
-      <c r="G35" s="30"/>
-      <c r="H35" s="30"/>
-      <c r="I35" s="30"/>
-      <c r="J35" s="31"/>
+        <v>63</v>
+      </c>
+      <c r="F35" s="28">
+        <v>45313</v>
+      </c>
+      <c r="G35" s="29" t="s">
+        <v>249</v>
+      </c>
+      <c r="H35" s="30" t="s">
+        <v>248</v>
+      </c>
+      <c r="I35" s="30" t="s">
+        <v>114</v>
+      </c>
+      <c r="J35" s="31" t="s">
+        <v>66</v>
+      </c>
       <c r="K35" s="31"/>
       <c r="L35" s="31" t="s">
         <v>98</v>
@@ -3633,13 +3651,13 @@
         <v>66</v>
       </c>
       <c r="N35" s="31" t="s">
-        <v>118</v>
+        <v>116</v>
       </c>
       <c r="O35" s="31" t="s">
         <v>66</v>
       </c>
       <c r="P35" s="31" t="s">
-        <v>117</v>
+        <v>130</v>
       </c>
       <c r="Q35" s="31"/>
       <c r="R35" s="32"/>
@@ -3650,7 +3668,7 @@
     </row>
     <row r="36" spans="1:20" s="46" customFormat="1" ht="20.100000000000001" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A36" s="25">
-        <v>75</v>
+        <v>47</v>
       </c>
       <c r="B36" s="26" t="s">
         <v>44</v>
@@ -3659,26 +3677,32 @@
         <v>57</v>
       </c>
       <c r="D36" s="26" t="s">
-        <v>155</v>
+        <v>154</v>
       </c>
       <c r="E36" s="27" t="s">
-        <v>156</v>
+        <v>65</v>
       </c>
       <c r="F36" s="28"/>
       <c r="G36" s="30"/>
       <c r="H36" s="30"/>
       <c r="I36" s="30"/>
-      <c r="J36" s="31" t="s">
+      <c r="J36" s="31"/>
+      <c r="K36" s="31"/>
+      <c r="L36" s="31" t="s">
         <v>98</v>
       </c>
-      <c r="K36" s="24" t="s">
-        <v>250</v>
-      </c>
-      <c r="L36" s="31"/>
-      <c r="M36" s="31"/>
-      <c r="N36" s="31"/>
-      <c r="O36" s="31"/>
-      <c r="P36" s="31"/>
+      <c r="M36" s="31" t="s">
+        <v>66</v>
+      </c>
+      <c r="N36" s="31" t="s">
+        <v>118</v>
+      </c>
+      <c r="O36" s="31" t="s">
+        <v>66</v>
+      </c>
+      <c r="P36" s="31" t="s">
+        <v>117</v>
+      </c>
       <c r="Q36" s="31"/>
       <c r="R36" s="32"/>
       <c r="S36" s="33"/>
@@ -3688,7 +3712,7 @@
     </row>
     <row r="37" spans="1:20" s="46" customFormat="1" ht="20.100000000000001" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A37" s="25">
-        <v>76</v>
+        <v>75</v>
       </c>
       <c r="B37" s="26" t="s">
         <v>44</v>
@@ -3697,20 +3721,20 @@
         <v>57</v>
       </c>
       <c r="D37" s="26" t="s">
-        <v>157</v>
+        <v>155</v>
       </c>
       <c r="E37" s="27" t="s">
-        <v>158</v>
+        <v>156</v>
       </c>
       <c r="F37" s="28"/>
       <c r="G37" s="30"/>
       <c r="H37" s="30"/>
       <c r="I37" s="30"/>
-      <c r="J37" s="41" t="s">
+      <c r="J37" s="31" t="s">
         <v>98</v>
       </c>
       <c r="K37" s="24" t="s">
-        <v>251</v>
+        <v>250</v>
       </c>
       <c r="L37" s="31"/>
       <c r="M37" s="31"/>
@@ -3726,7 +3750,7 @@
     </row>
     <row r="38" spans="1:20" s="46" customFormat="1" ht="20.100000000000001" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A38" s="25">
-        <v>77</v>
+        <v>76</v>
       </c>
       <c r="B38" s="26" t="s">
         <v>44</v>
@@ -3735,10 +3759,10 @@
         <v>57</v>
       </c>
       <c r="D38" s="26" t="s">
-        <v>159</v>
+        <v>157</v>
       </c>
       <c r="E38" s="27" t="s">
-        <v>160</v>
+        <v>158</v>
       </c>
       <c r="F38" s="28"/>
       <c r="G38" s="30"/>
@@ -3748,7 +3772,7 @@
         <v>98</v>
       </c>
       <c r="K38" s="24" t="s">
-        <v>252</v>
+        <v>251</v>
       </c>
       <c r="L38" s="31"/>
       <c r="M38" s="31"/>
@@ -3764,7 +3788,7 @@
     </row>
     <row r="39" spans="1:20" s="46" customFormat="1" ht="20.100000000000001" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A39" s="25">
-        <v>78</v>
+        <v>77</v>
       </c>
       <c r="B39" s="26" t="s">
         <v>44</v>
@@ -3773,10 +3797,10 @@
         <v>57</v>
       </c>
       <c r="D39" s="26" t="s">
-        <v>161</v>
+        <v>159</v>
       </c>
       <c r="E39" s="27" t="s">
-        <v>162</v>
+        <v>160</v>
       </c>
       <c r="F39" s="28"/>
       <c r="G39" s="30"/>
@@ -3786,7 +3810,7 @@
         <v>98</v>
       </c>
       <c r="K39" s="24" t="s">
-        <v>253</v>
+        <v>252</v>
       </c>
       <c r="L39" s="31"/>
       <c r="M39" s="31"/>
@@ -3802,7 +3826,7 @@
     </row>
     <row r="40" spans="1:20" s="46" customFormat="1" ht="20.100000000000001" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A40" s="25">
-        <v>79</v>
+        <v>78</v>
       </c>
       <c r="B40" s="26" t="s">
         <v>44</v>
@@ -3811,10 +3835,10 @@
         <v>57</v>
       </c>
       <c r="D40" s="26" t="s">
-        <v>163</v>
+        <v>161</v>
       </c>
       <c r="E40" s="27" t="s">
-        <v>164</v>
+        <v>162</v>
       </c>
       <c r="F40" s="28"/>
       <c r="G40" s="30"/>
@@ -3824,7 +3848,7 @@
         <v>98</v>
       </c>
       <c r="K40" s="24" t="s">
-        <v>254</v>
+        <v>253</v>
       </c>
       <c r="L40" s="31"/>
       <c r="M40" s="31"/>
@@ -3840,7 +3864,7 @@
     </row>
     <row r="41" spans="1:20" s="46" customFormat="1" ht="20.100000000000001" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A41" s="25">
-        <v>80</v>
+        <v>79</v>
       </c>
       <c r="B41" s="26" t="s">
         <v>44</v>
@@ -3849,10 +3873,10 @@
         <v>57</v>
       </c>
       <c r="D41" s="26" t="s">
-        <v>165</v>
+        <v>163</v>
       </c>
       <c r="E41" s="27" t="s">
-        <v>166</v>
+        <v>164</v>
       </c>
       <c r="F41" s="28"/>
       <c r="G41" s="30"/>
@@ -3862,7 +3886,7 @@
         <v>98</v>
       </c>
       <c r="K41" s="24" t="s">
-        <v>255</v>
+        <v>254</v>
       </c>
       <c r="L41" s="31"/>
       <c r="M41" s="31"/>
@@ -3878,7 +3902,7 @@
     </row>
     <row r="42" spans="1:20" s="46" customFormat="1" ht="20.100000000000001" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A42" s="25">
-        <v>81</v>
+        <v>80</v>
       </c>
       <c r="B42" s="26" t="s">
         <v>44</v>
@@ -3887,10 +3911,10 @@
         <v>57</v>
       </c>
       <c r="D42" s="26" t="s">
-        <v>167</v>
+        <v>165</v>
       </c>
       <c r="E42" s="27" t="s">
-        <v>168</v>
+        <v>166</v>
       </c>
       <c r="F42" s="28"/>
       <c r="G42" s="30"/>
@@ -3900,7 +3924,7 @@
         <v>98</v>
       </c>
       <c r="K42" s="24" t="s">
-        <v>256</v>
+        <v>255</v>
       </c>
       <c r="L42" s="31"/>
       <c r="M42" s="31"/>
@@ -3916,7 +3940,7 @@
     </row>
     <row r="43" spans="1:20" s="46" customFormat="1" ht="20.100000000000001" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A43" s="25">
-        <v>82</v>
+        <v>81</v>
       </c>
       <c r="B43" s="26" t="s">
         <v>44</v>
@@ -3925,20 +3949,20 @@
         <v>57</v>
       </c>
       <c r="D43" s="26" t="s">
-        <v>169</v>
+        <v>167</v>
       </c>
       <c r="E43" s="27" t="s">
-        <v>170</v>
+        <v>168</v>
       </c>
       <c r="F43" s="28"/>
       <c r="G43" s="30"/>
       <c r="H43" s="30"/>
       <c r="I43" s="30"/>
-      <c r="J43" s="31" t="s">
+      <c r="J43" s="41" t="s">
         <v>98</v>
       </c>
       <c r="K43" s="24" t="s">
-        <v>257</v>
+        <v>256</v>
       </c>
       <c r="L43" s="31"/>
       <c r="M43" s="31"/>
@@ -3954,7 +3978,7 @@
     </row>
     <row r="44" spans="1:20" s="46" customFormat="1" ht="20.100000000000001" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A44" s="25">
-        <v>83</v>
+        <v>82</v>
       </c>
       <c r="B44" s="26" t="s">
         <v>44</v>
@@ -3963,10 +3987,10 @@
         <v>57</v>
       </c>
       <c r="D44" s="26" t="s">
-        <v>171</v>
+        <v>169</v>
       </c>
       <c r="E44" s="27" t="s">
-        <v>172</v>
+        <v>170</v>
       </c>
       <c r="F44" s="28"/>
       <c r="G44" s="30"/>
@@ -3976,7 +4000,7 @@
         <v>98</v>
       </c>
       <c r="K44" s="24" t="s">
-        <v>258</v>
+        <v>257</v>
       </c>
       <c r="L44" s="31"/>
       <c r="M44" s="31"/>
@@ -3992,7 +4016,7 @@
     </row>
     <row r="45" spans="1:20" s="46" customFormat="1" ht="20.100000000000001" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A45" s="25">
-        <v>84</v>
+        <v>83</v>
       </c>
       <c r="B45" s="26" t="s">
         <v>44</v>
@@ -4001,19 +4025,19 @@
         <v>57</v>
       </c>
       <c r="D45" s="26" t="s">
-        <v>173</v>
+        <v>171</v>
       </c>
       <c r="E45" s="27" t="s">
-        <v>174</v>
+        <v>172</v>
       </c>
       <c r="F45" s="28"/>
       <c r="G45" s="30"/>
       <c r="H45" s="30"/>
       <c r="I45" s="30"/>
-      <c r="J45" s="47" t="s">
+      <c r="J45" s="48" t="s">
         <v>98</v>
       </c>
-      <c r="K45" s="31" t="s">
+      <c r="K45" s="24" t="s">
         <v>258</v>
       </c>
       <c r="L45" s="31"/>
@@ -4030,7 +4054,7 @@
     </row>
     <row r="46" spans="1:20" s="46" customFormat="1" ht="20.100000000000001" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A46" s="25">
-        <v>85</v>
+        <v>84</v>
       </c>
       <c r="B46" s="26" t="s">
         <v>44</v>
@@ -4039,42 +4063,26 @@
         <v>57</v>
       </c>
       <c r="D46" s="26" t="s">
-        <v>175</v>
+        <v>173</v>
       </c>
       <c r="E46" s="27" t="s">
-        <v>176</v>
-      </c>
-      <c r="F46" s="28">
-        <v>45313</v>
-      </c>
-      <c r="G46" s="29" t="s">
-        <v>261</v>
-      </c>
-      <c r="H46" s="30" t="s">
-        <v>260</v>
-      </c>
-      <c r="I46" s="30" t="s">
-        <v>262</v>
-      </c>
-      <c r="J46" s="48" t="s">
-        <v>66</v>
-      </c>
-      <c r="K46" s="31"/>
-      <c r="L46" s="31" t="s">
-        <v>66</v>
-      </c>
-      <c r="M46" s="31" t="s">
-        <v>66</v>
-      </c>
-      <c r="N46" s="31" t="s">
-        <v>263</v>
-      </c>
-      <c r="O46" s="31" t="s">
-        <v>66</v>
-      </c>
-      <c r="P46" s="31" t="s">
-        <v>130</v>
-      </c>
+        <v>174</v>
+      </c>
+      <c r="F46" s="28"/>
+      <c r="G46" s="30"/>
+      <c r="H46" s="30"/>
+      <c r="I46" s="30"/>
+      <c r="J46" s="47" t="s">
+        <v>98</v>
+      </c>
+      <c r="K46" s="31" t="s">
+        <v>258</v>
+      </c>
+      <c r="L46" s="31"/>
+      <c r="M46" s="31"/>
+      <c r="N46" s="31"/>
+      <c r="O46" s="31"/>
+      <c r="P46" s="31"/>
       <c r="Q46" s="31"/>
       <c r="R46" s="32"/>
       <c r="S46" s="33"/>
@@ -4084,7 +4092,7 @@
     </row>
     <row r="47" spans="1:20" s="46" customFormat="1" ht="20.100000000000001" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A47" s="25">
-        <v>86</v>
+        <v>85</v>
       </c>
       <c r="B47" s="26" t="s">
         <v>44</v>
@@ -4093,26 +4101,42 @@
         <v>57</v>
       </c>
       <c r="D47" s="26" t="s">
-        <v>177</v>
+        <v>175</v>
       </c>
       <c r="E47" s="27" t="s">
-        <v>178</v>
-      </c>
-      <c r="F47" s="28"/>
-      <c r="G47" s="30"/>
-      <c r="H47" s="30"/>
-      <c r="I47" s="30"/>
-      <c r="J47" s="41" t="s">
-        <v>98</v>
-      </c>
-      <c r="K47" s="31" t="s">
-        <v>259</v>
-      </c>
-      <c r="L47" s="31"/>
-      <c r="M47" s="31"/>
-      <c r="N47" s="31"/>
-      <c r="O47" s="31"/>
-      <c r="P47" s="31"/>
+        <v>176</v>
+      </c>
+      <c r="F47" s="28">
+        <v>45313</v>
+      </c>
+      <c r="G47" s="29" t="s">
+        <v>261</v>
+      </c>
+      <c r="H47" s="30" t="s">
+        <v>260</v>
+      </c>
+      <c r="I47" s="30" t="s">
+        <v>262</v>
+      </c>
+      <c r="J47" s="31" t="s">
+        <v>66</v>
+      </c>
+      <c r="K47" s="31"/>
+      <c r="L47" s="31" t="s">
+        <v>66</v>
+      </c>
+      <c r="M47" s="31" t="s">
+        <v>66</v>
+      </c>
+      <c r="N47" s="31" t="s">
+        <v>263</v>
+      </c>
+      <c r="O47" s="31" t="s">
+        <v>66</v>
+      </c>
+      <c r="P47" s="31" t="s">
+        <v>130</v>
+      </c>
       <c r="Q47" s="31"/>
       <c r="R47" s="32"/>
       <c r="S47" s="33"/>
@@ -4122,7 +4146,7 @@
     </row>
     <row r="48" spans="1:20" s="46" customFormat="1" ht="20.100000000000001" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A48" s="25">
-        <v>87</v>
+        <v>86</v>
       </c>
       <c r="B48" s="26" t="s">
         <v>44</v>
@@ -4131,16 +4155,16 @@
         <v>57</v>
       </c>
       <c r="D48" s="26" t="s">
-        <v>179</v>
+        <v>177</v>
       </c>
       <c r="E48" s="27" t="s">
-        <v>180</v>
+        <v>178</v>
       </c>
       <c r="F48" s="28"/>
       <c r="G48" s="30"/>
       <c r="H48" s="30"/>
       <c r="I48" s="30"/>
-      <c r="J48" s="31" t="s">
+      <c r="J48" s="41" t="s">
         <v>98</v>
       </c>
       <c r="K48" s="31" t="s">
@@ -4160,7 +4184,7 @@
     </row>
     <row r="49" spans="1:20" s="46" customFormat="1" ht="20.100000000000001" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A49" s="25">
-        <v>88</v>
+        <v>87</v>
       </c>
       <c r="B49" s="26" t="s">
         <v>44</v>
@@ -4169,10 +4193,10 @@
         <v>57</v>
       </c>
       <c r="D49" s="26" t="s">
-        <v>181</v>
+        <v>179</v>
       </c>
       <c r="E49" s="27" t="s">
-        <v>182</v>
+        <v>180</v>
       </c>
       <c r="F49" s="28"/>
       <c r="G49" s="30"/>
@@ -4198,7 +4222,7 @@
     </row>
     <row r="50" spans="1:20" s="46" customFormat="1" ht="20.100000000000001" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A50" s="25">
-        <v>89</v>
+        <v>88</v>
       </c>
       <c r="B50" s="26" t="s">
         <v>44</v>
@@ -4207,10 +4231,10 @@
         <v>57</v>
       </c>
       <c r="D50" s="26" t="s">
-        <v>183</v>
+        <v>181</v>
       </c>
       <c r="E50" s="27" t="s">
-        <v>184</v>
+        <v>182</v>
       </c>
       <c r="F50" s="28"/>
       <c r="G50" s="30"/>
@@ -4236,7 +4260,7 @@
     </row>
     <row r="51" spans="1:20" s="46" customFormat="1" ht="20.100000000000001" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A51" s="25">
-        <v>90</v>
+        <v>89</v>
       </c>
       <c r="B51" s="26" t="s">
         <v>44</v>
@@ -4245,10 +4269,10 @@
         <v>57</v>
       </c>
       <c r="D51" s="26" t="s">
-        <v>185</v>
+        <v>183</v>
       </c>
       <c r="E51" s="27" t="s">
-        <v>186</v>
+        <v>184</v>
       </c>
       <c r="F51" s="28"/>
       <c r="G51" s="30"/>
@@ -4274,7 +4298,7 @@
     </row>
     <row r="52" spans="1:20" s="46" customFormat="1" ht="20.100000000000001" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A52" s="25">
-        <v>91</v>
+        <v>90</v>
       </c>
       <c r="B52" s="26" t="s">
         <v>44</v>
@@ -4283,10 +4307,10 @@
         <v>57</v>
       </c>
       <c r="D52" s="26" t="s">
-        <v>187</v>
+        <v>185</v>
       </c>
       <c r="E52" s="27" t="s">
-        <v>188</v>
+        <v>186</v>
       </c>
       <c r="F52" s="28"/>
       <c r="G52" s="30"/>
@@ -4312,7 +4336,7 @@
     </row>
     <row r="53" spans="1:20" s="46" customFormat="1" ht="20.100000000000001" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A53" s="25">
-        <v>92</v>
+        <v>91</v>
       </c>
       <c r="B53" s="26" t="s">
         <v>44</v>
@@ -4321,10 +4345,10 @@
         <v>57</v>
       </c>
       <c r="D53" s="26" t="s">
-        <v>189</v>
+        <v>187</v>
       </c>
       <c r="E53" s="27" t="s">
-        <v>190</v>
+        <v>188</v>
       </c>
       <c r="F53" s="28"/>
       <c r="G53" s="30"/>
@@ -4350,7 +4374,7 @@
     </row>
     <row r="54" spans="1:20" s="46" customFormat="1" ht="20.100000000000001" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A54" s="25">
-        <v>93</v>
+        <v>92</v>
       </c>
       <c r="B54" s="26" t="s">
         <v>44</v>
@@ -4359,10 +4383,10 @@
         <v>57</v>
       </c>
       <c r="D54" s="26" t="s">
-        <v>191</v>
+        <v>189</v>
       </c>
       <c r="E54" s="27" t="s">
-        <v>192</v>
+        <v>190</v>
       </c>
       <c r="F54" s="28"/>
       <c r="G54" s="30"/>
@@ -4388,51 +4412,35 @@
     </row>
     <row r="55" spans="1:20" s="46" customFormat="1" ht="20.100000000000001" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A55" s="25">
-        <v>32</v>
+        <v>93</v>
       </c>
       <c r="B55" s="26" t="s">
         <v>44</v>
       </c>
       <c r="C55" s="26" t="s">
-        <v>61</v>
+        <v>57</v>
       </c>
       <c r="D55" s="26" t="s">
-        <v>193</v>
+        <v>191</v>
       </c>
       <c r="E55" s="27" t="s">
-        <v>59</v>
-      </c>
-      <c r="F55" s="28">
-        <v>45313</v>
-      </c>
-      <c r="G55" s="29" t="s">
-        <v>268</v>
-      </c>
-      <c r="H55" s="30" t="s">
-        <v>267</v>
-      </c>
-      <c r="I55" s="30" t="s">
-        <v>114</v>
-      </c>
+        <v>192</v>
+      </c>
+      <c r="F55" s="28"/>
+      <c r="G55" s="30"/>
+      <c r="H55" s="30"/>
+      <c r="I55" s="30"/>
       <c r="J55" s="31" t="s">
-        <v>66</v>
-      </c>
-      <c r="K55" s="31"/>
-      <c r="L55" s="31" t="s">
         <v>98</v>
       </c>
-      <c r="M55" s="31" t="s">
-        <v>66</v>
-      </c>
-      <c r="N55" s="31" t="s">
-        <v>115</v>
-      </c>
-      <c r="O55" s="31" t="s">
-        <v>66</v>
-      </c>
-      <c r="P55" s="31" t="s">
-        <v>130</v>
-      </c>
+      <c r="K55" s="31" t="s">
+        <v>259</v>
+      </c>
+      <c r="L55" s="31"/>
+      <c r="M55" s="31"/>
+      <c r="N55" s="31"/>
+      <c r="O55" s="31"/>
+      <c r="P55" s="31"/>
       <c r="Q55" s="31"/>
       <c r="R55" s="32"/>
       <c r="S55" s="33"/>
@@ -4442,7 +4450,7 @@
     </row>
     <row r="56" spans="1:20" s="46" customFormat="1" ht="20.100000000000001" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A56" s="25">
-        <v>40</v>
+        <v>32</v>
       </c>
       <c r="B56" s="26" t="s">
         <v>44</v>
@@ -4451,25 +4459,25 @@
         <v>61</v>
       </c>
       <c r="D56" s="26" t="s">
-        <v>194</v>
+        <v>193</v>
       </c>
       <c r="E56" s="27" t="s">
-        <v>63</v>
+        <v>59</v>
       </c>
       <c r="F56" s="28">
         <v>45313</v>
       </c>
       <c r="G56" s="29" t="s">
-        <v>271</v>
+        <v>268</v>
       </c>
       <c r="H56" s="30" t="s">
-        <v>270</v>
+        <v>267</v>
       </c>
       <c r="I56" s="30" t="s">
         <v>114</v>
       </c>
       <c r="J56" s="31" t="s">
-        <v>269</v>
+        <v>66</v>
       </c>
       <c r="K56" s="31"/>
       <c r="L56" s="31" t="s">
@@ -4479,7 +4487,7 @@
         <v>66</v>
       </c>
       <c r="N56" s="31" t="s">
-        <v>116</v>
+        <v>115</v>
       </c>
       <c r="O56" s="31" t="s">
         <v>66</v>
@@ -4496,7 +4504,7 @@
     </row>
     <row r="57" spans="1:20" s="46" customFormat="1" ht="20.100000000000001" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A57" s="25">
-        <v>48</v>
+        <v>40</v>
       </c>
       <c r="B57" s="26" t="s">
         <v>44</v>
@@ -4505,16 +4513,26 @@
         <v>61</v>
       </c>
       <c r="D57" s="26" t="s">
-        <v>195</v>
+        <v>194</v>
       </c>
       <c r="E57" s="27" t="s">
-        <v>65</v>
-      </c>
-      <c r="F57" s="28"/>
-      <c r="G57" s="30"/>
-      <c r="H57" s="30"/>
-      <c r="I57" s="30"/>
-      <c r="J57" s="31"/>
+        <v>63</v>
+      </c>
+      <c r="F57" s="28">
+        <v>45313</v>
+      </c>
+      <c r="G57" s="29" t="s">
+        <v>271</v>
+      </c>
+      <c r="H57" s="30" t="s">
+        <v>270</v>
+      </c>
+      <c r="I57" s="30" t="s">
+        <v>114</v>
+      </c>
+      <c r="J57" s="31" t="s">
+        <v>269</v>
+      </c>
       <c r="K57" s="31"/>
       <c r="L57" s="31" t="s">
         <v>98</v>
@@ -4523,13 +4541,13 @@
         <v>66</v>
       </c>
       <c r="N57" s="31" t="s">
-        <v>118</v>
+        <v>116</v>
       </c>
       <c r="O57" s="31" t="s">
         <v>66</v>
       </c>
       <c r="P57" s="31" t="s">
-        <v>117</v>
+        <v>130</v>
       </c>
       <c r="Q57" s="31"/>
       <c r="R57" s="32"/>
@@ -4539,8 +4557,8 @@
       </c>
     </row>
     <row r="58" spans="1:20" s="46" customFormat="1" ht="20.100000000000001" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A58" s="49">
-        <v>147</v>
+      <c r="A58" s="25">
+        <v>48</v>
       </c>
       <c r="B58" s="26" t="s">
         <v>44</v>
@@ -4549,42 +4567,42 @@
         <v>61</v>
       </c>
       <c r="D58" s="26" t="s">
-        <v>196</v>
+        <v>195</v>
       </c>
       <c r="E58" s="27" t="s">
-        <v>197</v>
-      </c>
-      <c r="F58" s="28">
-        <v>45313</v>
-      </c>
-      <c r="G58" s="29" t="s">
-        <v>266</v>
-      </c>
-      <c r="H58" s="30" t="s">
-        <v>265</v>
-      </c>
-      <c r="I58" s="30" t="s">
-        <v>264</v>
-      </c>
-      <c r="J58" s="31" t="s">
+        <v>65</v>
+      </c>
+      <c r="F58" s="28"/>
+      <c r="G58" s="30"/>
+      <c r="H58" s="30"/>
+      <c r="I58" s="30"/>
+      <c r="J58" s="31"/>
+      <c r="K58" s="31"/>
+      <c r="L58" s="31" t="s">
+        <v>98</v>
+      </c>
+      <c r="M58" s="31" t="s">
         <v>66</v>
       </c>
-      <c r="K58" s="31"/>
-      <c r="L58" s="31"/>
-      <c r="M58" s="31"/>
-      <c r="N58" s="31"/>
-      <c r="O58" s="31"/>
-      <c r="P58" s="31"/>
+      <c r="N58" s="31" t="s">
+        <v>118</v>
+      </c>
+      <c r="O58" s="31" t="s">
+        <v>66</v>
+      </c>
+      <c r="P58" s="31" t="s">
+        <v>117</v>
+      </c>
       <c r="Q58" s="31"/>
       <c r="R58" s="32"/>
       <c r="S58" s="33"/>
       <c r="T58" s="34" t="s">
-        <v>48</v>
+        <v>60</v>
       </c>
     </row>
     <row r="59" spans="1:20" s="46" customFormat="1" ht="20.100000000000001" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A59" s="49">
-        <v>148</v>
+        <v>147</v>
       </c>
       <c r="B59" s="26" t="s">
         <v>44</v>
@@ -4593,21 +4611,27 @@
         <v>61</v>
       </c>
       <c r="D59" s="26" t="s">
-        <v>198</v>
+        <v>196</v>
       </c>
       <c r="E59" s="27" t="s">
-        <v>199</v>
-      </c>
-      <c r="F59" s="28"/>
-      <c r="G59" s="30"/>
-      <c r="H59" s="30"/>
-      <c r="I59" s="30"/>
+        <v>197</v>
+      </c>
+      <c r="F59" s="28">
+        <v>45313</v>
+      </c>
+      <c r="G59" s="29" t="s">
+        <v>266</v>
+      </c>
+      <c r="H59" s="30" t="s">
+        <v>265</v>
+      </c>
+      <c r="I59" s="30" t="s">
+        <v>264</v>
+      </c>
       <c r="J59" s="31" t="s">
-        <v>98</v>
-      </c>
-      <c r="K59" s="31" t="s">
-        <v>272</v>
-      </c>
+        <v>66</v>
+      </c>
+      <c r="K59" s="31"/>
       <c r="L59" s="31"/>
       <c r="M59" s="31"/>
       <c r="N59" s="31"/>
@@ -4622,7 +4646,7 @@
     </row>
     <row r="60" spans="1:20" s="46" customFormat="1" ht="20.100000000000001" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A60" s="49">
-        <v>149</v>
+        <v>148</v>
       </c>
       <c r="B60" s="26" t="s">
         <v>44</v>
@@ -4631,10 +4655,10 @@
         <v>61</v>
       </c>
       <c r="D60" s="26" t="s">
-        <v>200</v>
+        <v>198</v>
       </c>
       <c r="E60" s="27" t="s">
-        <v>201</v>
+        <v>199</v>
       </c>
       <c r="F60" s="28"/>
       <c r="G60" s="30"/>
@@ -4644,7 +4668,7 @@
         <v>98</v>
       </c>
       <c r="K60" s="31" t="s">
-        <v>273</v>
+        <v>272</v>
       </c>
       <c r="L60" s="31"/>
       <c r="M60" s="31"/>
@@ -4660,7 +4684,7 @@
     </row>
     <row r="61" spans="1:20" s="46" customFormat="1" ht="20.100000000000001" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A61" s="49">
-        <v>150</v>
+        <v>149</v>
       </c>
       <c r="B61" s="26" t="s">
         <v>44</v>
@@ -4669,10 +4693,10 @@
         <v>61</v>
       </c>
       <c r="D61" s="26" t="s">
-        <v>202</v>
+        <v>200</v>
       </c>
       <c r="E61" s="27" t="s">
-        <v>203</v>
+        <v>201</v>
       </c>
       <c r="F61" s="28"/>
       <c r="G61" s="30"/>
@@ -4682,7 +4706,7 @@
         <v>98</v>
       </c>
       <c r="K61" s="31" t="s">
-        <v>274</v>
+        <v>273</v>
       </c>
       <c r="L61" s="31"/>
       <c r="M61" s="31"/>
@@ -4697,8 +4721,8 @@
       </c>
     </row>
     <row r="62" spans="1:20" s="46" customFormat="1" ht="20.100000000000001" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A62" s="25">
-        <v>151</v>
+      <c r="A62" s="49">
+        <v>150</v>
       </c>
       <c r="B62" s="26" t="s">
         <v>44</v>
@@ -4707,22 +4731,22 @@
         <v>61</v>
       </c>
       <c r="D62" s="26" t="s">
-        <v>204</v>
+        <v>202</v>
       </c>
       <c r="E62" s="27" t="s">
-        <v>205</v>
+        <v>203</v>
       </c>
       <c r="F62" s="28"/>
       <c r="G62" s="30"/>
       <c r="H62" s="30"/>
       <c r="I62" s="30"/>
-      <c r="J62" s="41" t="s">
+      <c r="J62" s="31" t="s">
         <v>98</v>
       </c>
       <c r="K62" s="31" t="s">
-        <v>275</v>
-      </c>
-      <c r="L62" s="41"/>
+        <v>274</v>
+      </c>
+      <c r="L62" s="31"/>
       <c r="M62" s="31"/>
       <c r="N62" s="31"/>
       <c r="O62" s="31"/>
@@ -4731,12 +4755,12 @@
       <c r="R62" s="32"/>
       <c r="S62" s="33"/>
       <c r="T62" s="34" t="s">
-        <v>60</v>
+        <v>48</v>
       </c>
     </row>
     <row r="63" spans="1:20" s="46" customFormat="1" ht="20.100000000000001" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A63" s="25">
-        <v>152</v>
+        <v>151</v>
       </c>
       <c r="B63" s="26" t="s">
         <v>44</v>
@@ -4745,22 +4769,22 @@
         <v>61</v>
       </c>
       <c r="D63" s="26" t="s">
-        <v>206</v>
+        <v>204</v>
       </c>
       <c r="E63" s="27" t="s">
-        <v>207</v>
+        <v>205</v>
       </c>
       <c r="F63" s="28"/>
       <c r="G63" s="30"/>
       <c r="H63" s="30"/>
       <c r="I63" s="30"/>
-      <c r="J63" s="31" t="s">
+      <c r="J63" s="41" t="s">
         <v>98</v>
       </c>
       <c r="K63" s="31" t="s">
-        <v>290</v>
-      </c>
-      <c r="L63" s="31"/>
+        <v>275</v>
+      </c>
+      <c r="L63" s="41"/>
       <c r="M63" s="31"/>
       <c r="N63" s="31"/>
       <c r="O63" s="31"/>
@@ -4774,7 +4798,7 @@
     </row>
     <row r="64" spans="1:20" s="46" customFormat="1" ht="20.100000000000001" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A64" s="25">
-        <v>153</v>
+        <v>152</v>
       </c>
       <c r="B64" s="26" t="s">
         <v>44</v>
@@ -4783,20 +4807,20 @@
         <v>61</v>
       </c>
       <c r="D64" s="26" t="s">
-        <v>208</v>
+        <v>206</v>
       </c>
       <c r="E64" s="27" t="s">
-        <v>209</v>
+        <v>207</v>
       </c>
       <c r="F64" s="28"/>
       <c r="G64" s="30"/>
       <c r="H64" s="30"/>
       <c r="I64" s="30"/>
-      <c r="J64" s="41" t="s">
+      <c r="J64" s="31" t="s">
         <v>98</v>
       </c>
       <c r="K64" s="31" t="s">
-        <v>276</v>
+        <v>290</v>
       </c>
       <c r="L64" s="31"/>
       <c r="M64" s="31"/>
@@ -4812,7 +4836,7 @@
     </row>
     <row r="65" spans="1:20" s="46" customFormat="1" ht="20.100000000000001" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A65" s="25">
-        <v>154</v>
+        <v>153</v>
       </c>
       <c r="B65" s="26" t="s">
         <v>44</v>
@@ -4821,10 +4845,10 @@
         <v>61</v>
       </c>
       <c r="D65" s="26" t="s">
-        <v>210</v>
+        <v>208</v>
       </c>
       <c r="E65" s="27" t="s">
-        <v>211</v>
+        <v>209</v>
       </c>
       <c r="F65" s="28"/>
       <c r="G65" s="30"/>
@@ -4833,8 +4857,8 @@
       <c r="J65" s="41" t="s">
         <v>98</v>
       </c>
-      <c r="K65" s="41" t="s">
-        <v>288</v>
+      <c r="K65" s="31" t="s">
+        <v>276</v>
       </c>
       <c r="L65" s="31"/>
       <c r="M65" s="31"/>
@@ -4850,7 +4874,7 @@
     </row>
     <row r="66" spans="1:20" s="46" customFormat="1" ht="20.100000000000001" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A66" s="25">
-        <v>155</v>
+        <v>154</v>
       </c>
       <c r="B66" s="26" t="s">
         <v>44</v>
@@ -4859,10 +4883,10 @@
         <v>61</v>
       </c>
       <c r="D66" s="26" t="s">
-        <v>212</v>
+        <v>210</v>
       </c>
       <c r="E66" s="27" t="s">
-        <v>213</v>
+        <v>211</v>
       </c>
       <c r="F66" s="28"/>
       <c r="G66" s="30"/>
@@ -4872,7 +4896,7 @@
         <v>98</v>
       </c>
       <c r="K66" s="41" t="s">
-        <v>289</v>
+        <v>288</v>
       </c>
       <c r="L66" s="31"/>
       <c r="M66" s="31"/>
@@ -4888,7 +4912,7 @@
     </row>
     <row r="67" spans="1:20" s="46" customFormat="1" ht="20.100000000000001" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A67" s="25">
-        <v>156</v>
+        <v>155</v>
       </c>
       <c r="B67" s="26" t="s">
         <v>44</v>
@@ -4897,20 +4921,20 @@
         <v>61</v>
       </c>
       <c r="D67" s="26" t="s">
-        <v>214</v>
+        <v>212</v>
       </c>
       <c r="E67" s="27" t="s">
-        <v>215</v>
+        <v>213</v>
       </c>
       <c r="F67" s="28"/>
       <c r="G67" s="30"/>
       <c r="H67" s="30"/>
       <c r="I67" s="30"/>
-      <c r="J67" s="31" t="s">
+      <c r="J67" s="41" t="s">
         <v>98</v>
       </c>
-      <c r="K67" s="31" t="s">
-        <v>291</v>
+      <c r="K67" s="41" t="s">
+        <v>289</v>
       </c>
       <c r="L67" s="31"/>
       <c r="M67" s="31"/>
@@ -4926,7 +4950,7 @@
     </row>
     <row r="68" spans="1:20" s="46" customFormat="1" ht="20.100000000000001" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A68" s="25">
-        <v>157</v>
+        <v>156</v>
       </c>
       <c r="B68" s="26" t="s">
         <v>44</v>
@@ -4935,20 +4959,20 @@
         <v>61</v>
       </c>
       <c r="D68" s="26" t="s">
-        <v>216</v>
+        <v>214</v>
       </c>
       <c r="E68" s="27" t="s">
-        <v>217</v>
+        <v>215</v>
       </c>
       <c r="F68" s="28"/>
       <c r="G68" s="30"/>
       <c r="H68" s="30"/>
       <c r="I68" s="30"/>
-      <c r="J68" s="41" t="s">
+      <c r="J68" s="31" t="s">
         <v>98</v>
       </c>
-      <c r="K68" s="41" t="s">
-        <v>279</v>
+      <c r="K68" s="31" t="s">
+        <v>291</v>
       </c>
       <c r="L68" s="31"/>
       <c r="M68" s="31"/>
@@ -4964,7 +4988,7 @@
     </row>
     <row r="69" spans="1:20" s="46" customFormat="1" ht="20.100000000000001" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A69" s="25">
-        <v>158</v>
+        <v>157</v>
       </c>
       <c r="B69" s="26" t="s">
         <v>44</v>
@@ -4973,10 +4997,10 @@
         <v>61</v>
       </c>
       <c r="D69" s="26" t="s">
-        <v>218</v>
+        <v>216</v>
       </c>
       <c r="E69" s="27" t="s">
-        <v>219</v>
+        <v>217</v>
       </c>
       <c r="F69" s="28"/>
       <c r="G69" s="30"/>
@@ -4986,7 +5010,7 @@
         <v>98</v>
       </c>
       <c r="K69" s="41" t="s">
-        <v>280</v>
+        <v>279</v>
       </c>
       <c r="L69" s="31"/>
       <c r="M69" s="31"/>
@@ -5002,7 +5026,7 @@
     </row>
     <row r="70" spans="1:20" s="46" customFormat="1" ht="20.100000000000001" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A70" s="25">
-        <v>159</v>
+        <v>158</v>
       </c>
       <c r="B70" s="26" t="s">
         <v>44</v>
@@ -5011,10 +5035,10 @@
         <v>61</v>
       </c>
       <c r="D70" s="26" t="s">
-        <v>220</v>
+        <v>218</v>
       </c>
       <c r="E70" s="27" t="s">
-        <v>221</v>
+        <v>219</v>
       </c>
       <c r="F70" s="28"/>
       <c r="G70" s="30"/>
@@ -5024,7 +5048,7 @@
         <v>98</v>
       </c>
       <c r="K70" s="41" t="s">
-        <v>281</v>
+        <v>280</v>
       </c>
       <c r="L70" s="31"/>
       <c r="M70" s="31"/>
@@ -5040,7 +5064,7 @@
     </row>
     <row r="71" spans="1:20" s="46" customFormat="1" ht="20.100000000000001" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A71" s="25">
-        <v>160</v>
+        <v>159</v>
       </c>
       <c r="B71" s="26" t="s">
         <v>44</v>
@@ -5049,10 +5073,10 @@
         <v>61</v>
       </c>
       <c r="D71" s="26" t="s">
-        <v>222</v>
+        <v>220</v>
       </c>
       <c r="E71" s="27" t="s">
-        <v>223</v>
+        <v>221</v>
       </c>
       <c r="F71" s="28"/>
       <c r="G71" s="30"/>
@@ -5062,7 +5086,7 @@
         <v>98</v>
       </c>
       <c r="K71" s="41" t="s">
-        <v>277</v>
+        <v>281</v>
       </c>
       <c r="L71" s="31"/>
       <c r="M71" s="31"/>
@@ -5078,7 +5102,7 @@
     </row>
     <row r="72" spans="1:20" s="46" customFormat="1" ht="20.100000000000001" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A72" s="25">
-        <v>161</v>
+        <v>160</v>
       </c>
       <c r="B72" s="26" t="s">
         <v>44</v>
@@ -5087,10 +5111,10 @@
         <v>61</v>
       </c>
       <c r="D72" s="26" t="s">
-        <v>224</v>
+        <v>222</v>
       </c>
       <c r="E72" s="27" t="s">
-        <v>225</v>
+        <v>223</v>
       </c>
       <c r="F72" s="28"/>
       <c r="G72" s="30"/>
@@ -5100,7 +5124,7 @@
         <v>98</v>
       </c>
       <c r="K72" s="41" t="s">
-        <v>282</v>
+        <v>277</v>
       </c>
       <c r="L72" s="31"/>
       <c r="M72" s="31"/>
@@ -5116,7 +5140,7 @@
     </row>
     <row r="73" spans="1:20" s="46" customFormat="1" ht="20.100000000000001" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A73" s="25">
-        <v>162</v>
+        <v>161</v>
       </c>
       <c r="B73" s="26" t="s">
         <v>44</v>
@@ -5125,10 +5149,10 @@
         <v>61</v>
       </c>
       <c r="D73" s="26" t="s">
-        <v>226</v>
+        <v>224</v>
       </c>
       <c r="E73" s="27" t="s">
-        <v>227</v>
+        <v>225</v>
       </c>
       <c r="F73" s="28"/>
       <c r="G73" s="30"/>
@@ -5138,7 +5162,7 @@
         <v>98</v>
       </c>
       <c r="K73" s="41" t="s">
-        <v>283</v>
+        <v>282</v>
       </c>
       <c r="L73" s="31"/>
       <c r="M73" s="31"/>
@@ -5154,7 +5178,7 @@
     </row>
     <row r="74" spans="1:20" s="46" customFormat="1" ht="20.100000000000001" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A74" s="25">
-        <v>163</v>
+        <v>162</v>
       </c>
       <c r="B74" s="26" t="s">
         <v>44</v>
@@ -5163,10 +5187,10 @@
         <v>61</v>
       </c>
       <c r="D74" s="26" t="s">
-        <v>228</v>
+        <v>226</v>
       </c>
       <c r="E74" s="27" t="s">
-        <v>229</v>
+        <v>227</v>
       </c>
       <c r="F74" s="28"/>
       <c r="G74" s="30"/>
@@ -5176,7 +5200,7 @@
         <v>98</v>
       </c>
       <c r="K74" s="41" t="s">
-        <v>278</v>
+        <v>283</v>
       </c>
       <c r="L74" s="31"/>
       <c r="M74" s="31"/>
@@ -5192,7 +5216,7 @@
     </row>
     <row r="75" spans="1:20" s="46" customFormat="1" ht="20.100000000000001" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A75" s="25">
-        <v>164</v>
+        <v>163</v>
       </c>
       <c r="B75" s="26" t="s">
         <v>44</v>
@@ -5201,10 +5225,10 @@
         <v>61</v>
       </c>
       <c r="D75" s="26" t="s">
-        <v>230</v>
+        <v>228</v>
       </c>
       <c r="E75" s="27" t="s">
-        <v>231</v>
+        <v>229</v>
       </c>
       <c r="F75" s="28"/>
       <c r="G75" s="30"/>
@@ -5214,7 +5238,7 @@
         <v>98</v>
       </c>
       <c r="K75" s="41" t="s">
-        <v>284</v>
+        <v>278</v>
       </c>
       <c r="L75" s="31"/>
       <c r="M75" s="31"/>
@@ -5230,7 +5254,7 @@
     </row>
     <row r="76" spans="1:20" s="46" customFormat="1" ht="20.100000000000001" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A76" s="25">
-        <v>165</v>
+        <v>164</v>
       </c>
       <c r="B76" s="26" t="s">
         <v>44</v>
@@ -5239,10 +5263,10 @@
         <v>61</v>
       </c>
       <c r="D76" s="26" t="s">
-        <v>232</v>
+        <v>230</v>
       </c>
       <c r="E76" s="27" t="s">
-        <v>233</v>
+        <v>231</v>
       </c>
       <c r="F76" s="28"/>
       <c r="G76" s="30"/>
@@ -5268,7 +5292,7 @@
     </row>
     <row r="77" spans="1:20" s="46" customFormat="1" ht="20.100000000000001" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A77" s="25">
-        <v>166</v>
+        <v>165</v>
       </c>
       <c r="B77" s="26" t="s">
         <v>44</v>
@@ -5277,10 +5301,10 @@
         <v>61</v>
       </c>
       <c r="D77" s="26" t="s">
-        <v>234</v>
+        <v>232</v>
       </c>
       <c r="E77" s="27" t="s">
-        <v>235</v>
+        <v>233</v>
       </c>
       <c r="F77" s="28"/>
       <c r="G77" s="30"/>
@@ -5290,7 +5314,7 @@
         <v>98</v>
       </c>
       <c r="K77" s="41" t="s">
-        <v>285</v>
+        <v>284</v>
       </c>
       <c r="L77" s="31"/>
       <c r="M77" s="31"/>
@@ -5306,7 +5330,7 @@
     </row>
     <row r="78" spans="1:20" s="46" customFormat="1" ht="20.100000000000001" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A78" s="25">
-        <v>167</v>
+        <v>166</v>
       </c>
       <c r="B78" s="26" t="s">
         <v>44</v>
@@ -5315,10 +5339,10 @@
         <v>61</v>
       </c>
       <c r="D78" s="26" t="s">
-        <v>236</v>
+        <v>234</v>
       </c>
       <c r="E78" s="27" t="s">
-        <v>237</v>
+        <v>235</v>
       </c>
       <c r="F78" s="28"/>
       <c r="G78" s="30"/>
@@ -5344,7 +5368,7 @@
     </row>
     <row r="79" spans="1:20" s="46" customFormat="1" ht="20.100000000000001" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A79" s="25">
-        <v>168</v>
+        <v>167</v>
       </c>
       <c r="B79" s="26" t="s">
         <v>44</v>
@@ -5353,10 +5377,10 @@
         <v>61</v>
       </c>
       <c r="D79" s="26" t="s">
-        <v>238</v>
+        <v>236</v>
       </c>
       <c r="E79" s="27" t="s">
-        <v>239</v>
+        <v>237</v>
       </c>
       <c r="F79" s="28"/>
       <c r="G79" s="30"/>
@@ -5366,7 +5390,7 @@
         <v>98</v>
       </c>
       <c r="K79" s="41" t="s">
-        <v>286</v>
+        <v>285</v>
       </c>
       <c r="L79" s="31"/>
       <c r="M79" s="31"/>
@@ -5380,9 +5404,9 @@
         <v>60</v>
       </c>
     </row>
-    <row r="80" spans="1:20" s="46" customFormat="1" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="80" spans="1:20" s="46" customFormat="1" ht="20.100000000000001" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A80" s="25">
-        <v>169</v>
+        <v>168</v>
       </c>
       <c r="B80" s="26" t="s">
         <v>44</v>
@@ -5391,10 +5415,10 @@
         <v>61</v>
       </c>
       <c r="D80" s="26" t="s">
-        <v>240</v>
+        <v>238</v>
       </c>
       <c r="E80" s="27" t="s">
-        <v>241</v>
+        <v>239</v>
       </c>
       <c r="F80" s="28"/>
       <c r="G80" s="30"/>
@@ -5404,7 +5428,7 @@
         <v>98</v>
       </c>
       <c r="K80" s="41" t="s">
-        <v>287</v>
+        <v>286</v>
       </c>
       <c r="L80" s="31"/>
       <c r="M80" s="31"/>
@@ -5418,24 +5442,45 @@
         <v>60</v>
       </c>
     </row>
-    <row r="81" spans="6:20" x14ac:dyDescent="0.25">
-      <c r="F81" s="12"/>
-      <c r="G81" s="12"/>
-      <c r="H81" s="12"/>
-      <c r="I81" s="12"/>
-      <c r="J81" s="13"/>
-      <c r="K81" s="13"/>
-      <c r="L81" s="13"/>
-      <c r="M81" s="13"/>
-      <c r="N81" s="13"/>
-      <c r="O81" s="13"/>
-      <c r="P81" s="13"/>
-      <c r="Q81" s="13"/>
-      <c r="R81" s="14"/>
-      <c r="S81" s="2"/>
-      <c r="T81" s="15"/>
-    </row>
-    <row r="82" spans="6:20" x14ac:dyDescent="0.25">
+    <row r="81" spans="1:20" ht="34.5" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A81" s="25">
+        <v>169</v>
+      </c>
+      <c r="B81" s="26" t="s">
+        <v>44</v>
+      </c>
+      <c r="C81" s="26" t="s">
+        <v>61</v>
+      </c>
+      <c r="D81" s="26" t="s">
+        <v>240</v>
+      </c>
+      <c r="E81" s="27" t="s">
+        <v>241</v>
+      </c>
+      <c r="F81" s="28"/>
+      <c r="G81" s="30"/>
+      <c r="H81" s="30"/>
+      <c r="I81" s="30"/>
+      <c r="J81" s="41" t="s">
+        <v>98</v>
+      </c>
+      <c r="K81" s="41" t="s">
+        <v>287</v>
+      </c>
+      <c r="L81" s="31"/>
+      <c r="M81" s="31"/>
+      <c r="N81" s="31"/>
+      <c r="O81" s="31"/>
+      <c r="P81" s="31"/>
+      <c r="Q81" s="31"/>
+      <c r="R81" s="32"/>
+      <c r="S81" s="33"/>
+      <c r="T81" s="34" t="s">
+        <v>60</v>
+      </c>
+    </row>
+    <row r="82" spans="1:20" x14ac:dyDescent="0.25">
       <c r="F82" s="12"/>
       <c r="G82" s="12"/>
       <c r="H82" s="12"/>
@@ -5452,7 +5497,7 @@
       <c r="S82" s="2"/>
       <c r="T82" s="15"/>
     </row>
-    <row r="83" spans="6:20" x14ac:dyDescent="0.25">
+    <row r="83" spans="1:20" x14ac:dyDescent="0.25">
       <c r="F83" s="12"/>
       <c r="G83" s="12"/>
       <c r="H83" s="12"/>
@@ -5469,7 +5514,7 @@
       <c r="S83" s="2"/>
       <c r="T83" s="15"/>
     </row>
-    <row r="84" spans="6:20" x14ac:dyDescent="0.25">
+    <row r="84" spans="1:20" x14ac:dyDescent="0.25">
       <c r="F84" s="12"/>
       <c r="G84" s="12"/>
       <c r="H84" s="12"/>
@@ -5486,7 +5531,7 @@
       <c r="S84" s="2"/>
       <c r="T84" s="15"/>
     </row>
-    <row r="85" spans="6:20" x14ac:dyDescent="0.25">
+    <row r="85" spans="1:20" x14ac:dyDescent="0.25">
       <c r="F85" s="12"/>
       <c r="G85" s="12"/>
       <c r="H85" s="12"/>
@@ -5503,7 +5548,7 @@
       <c r="S85" s="2"/>
       <c r="T85" s="15"/>
     </row>
-    <row r="86" spans="6:20" x14ac:dyDescent="0.25">
+    <row r="86" spans="1:20" x14ac:dyDescent="0.25">
       <c r="F86" s="12"/>
       <c r="G86" s="12"/>
       <c r="H86" s="12"/>
@@ -5520,7 +5565,7 @@
       <c r="S86" s="2"/>
       <c r="T86" s="15"/>
     </row>
-    <row r="87" spans="6:20" x14ac:dyDescent="0.25">
+    <row r="87" spans="1:20" x14ac:dyDescent="0.25">
       <c r="F87" s="12"/>
       <c r="G87" s="12"/>
       <c r="H87" s="12"/>
@@ -5537,7 +5582,7 @@
       <c r="S87" s="2"/>
       <c r="T87" s="15"/>
     </row>
-    <row r="88" spans="6:20" x14ac:dyDescent="0.25">
+    <row r="88" spans="1:20" x14ac:dyDescent="0.25">
       <c r="F88" s="12"/>
       <c r="G88" s="12"/>
       <c r="H88" s="12"/>
@@ -5554,7 +5599,7 @@
       <c r="S88" s="2"/>
       <c r="T88" s="15"/>
     </row>
-    <row r="89" spans="6:20" x14ac:dyDescent="0.25">
+    <row r="89" spans="1:20" x14ac:dyDescent="0.25">
       <c r="F89" s="12"/>
       <c r="G89" s="12"/>
       <c r="H89" s="12"/>
@@ -5571,7 +5616,7 @@
       <c r="S89" s="2"/>
       <c r="T89" s="15"/>
     </row>
-    <row r="90" spans="6:20" x14ac:dyDescent="0.25">
+    <row r="90" spans="1:20" x14ac:dyDescent="0.25">
       <c r="F90" s="12"/>
       <c r="G90" s="12"/>
       <c r="H90" s="12"/>
@@ -5588,7 +5633,7 @@
       <c r="S90" s="2"/>
       <c r="T90" s="15"/>
     </row>
-    <row r="91" spans="6:20" x14ac:dyDescent="0.25">
+    <row r="91" spans="1:20" x14ac:dyDescent="0.25">
       <c r="F91" s="12"/>
       <c r="G91" s="12"/>
       <c r="H91" s="12"/>
@@ -5605,7 +5650,7 @@
       <c r="S91" s="2"/>
       <c r="T91" s="15"/>
     </row>
-    <row r="92" spans="6:20" x14ac:dyDescent="0.25">
+    <row r="92" spans="1:20" x14ac:dyDescent="0.25">
       <c r="F92" s="12"/>
       <c r="G92" s="12"/>
       <c r="H92" s="12"/>
@@ -5622,7 +5667,7 @@
       <c r="S92" s="2"/>
       <c r="T92" s="15"/>
     </row>
-    <row r="93" spans="6:20" x14ac:dyDescent="0.25">
+    <row r="93" spans="1:20" x14ac:dyDescent="0.25">
       <c r="F93" s="12"/>
       <c r="G93" s="12"/>
       <c r="H93" s="12"/>
@@ -5639,7 +5684,7 @@
       <c r="S93" s="2"/>
       <c r="T93" s="15"/>
     </row>
-    <row r="94" spans="6:20" x14ac:dyDescent="0.25">
+    <row r="94" spans="1:20" x14ac:dyDescent="0.25">
       <c r="F94" s="12"/>
       <c r="G94" s="12"/>
       <c r="H94" s="12"/>
@@ -5656,7 +5701,7 @@
       <c r="S94" s="2"/>
       <c r="T94" s="15"/>
     </row>
-    <row r="95" spans="6:20" x14ac:dyDescent="0.25">
+    <row r="95" spans="1:20" x14ac:dyDescent="0.25">
       <c r="F95" s="12"/>
       <c r="G95" s="12"/>
       <c r="H95" s="12"/>
@@ -5673,7 +5718,7 @@
       <c r="S95" s="2"/>
       <c r="T95" s="15"/>
     </row>
-    <row r="96" spans="6:20" x14ac:dyDescent="0.25">
+    <row r="96" spans="1:20" x14ac:dyDescent="0.25">
       <c r="F96" s="12"/>
       <c r="G96" s="12"/>
       <c r="H96" s="12"/>
@@ -9136,7 +9181,7 @@
     </row>
   </sheetData>
   <autoFilter ref="A9:T80" xr:uid="{00000000-0009-0000-0000-000002000000}">
-    <sortState xmlns:xlrd2="http://schemas.microsoft.com/office/spreadsheetml/2017/richdata2" ref="A10:T80">
+    <sortState xmlns:xlrd2="http://schemas.microsoft.com/office/spreadsheetml/2017/richdata2" ref="A10:T81">
       <sortCondition ref="C9:C80"/>
     </sortState>
   </autoFilter>

</xml_diff>

<commit_message>
FIX Razionale applicabilità testcase84
</commit_message>
<xml_diff>
--- a/GATEWAY/A1#111PROACTIVEXX/Proactive/Labpro/5.0/report-checklist.xlsx
+++ b/GATEWAY/A1#111PROACTIVEXX/Proactive/Labpro/5.0/report-checklist.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\vb_net_prj\API_REGIONETOSCANA\FSE 2.0\perValidazione\LAB+RAD+RSA\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{C64A4402-2534-4AA7-8E39-69E21A97CA1D}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{A9A255C9-7513-410A-ACE5-29E74AC4F639}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" activeTab="2" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -65,7 +65,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="656" uniqueCount="298">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="656" uniqueCount="299">
   <si>
     <t>COME VALORIZZARE LA CHECKLIST (tab TestCases)</t>
   </si>
@@ -1274,6 +1274,9 @@
   </si>
   <si>
     <t>20240124171704</t>
+  </si>
+  <si>
+    <t>Il software garantisce che il Codice dell'esame eseguito sia sempre valorizzato</t>
   </si>
 </sst>
 </file>
@@ -1369,7 +1372,7 @@
       <family val="2"/>
     </font>
   </fonts>
-  <fills count="7">
+  <fills count="8">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -1403,6 +1406,12 @@
     <fill>
       <patternFill patternType="solid">
         <fgColor theme="9" tint="0.79998168889431442"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="8" tint="0.59999389629810485"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -1658,7 +1667,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="74">
+  <cellXfs count="84">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
@@ -1786,36 +1795,11 @@
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
-    <xf numFmtId="0" fontId="10" fillId="0" borderId="19" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="19" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
-    <xf numFmtId="0" fontId="4" fillId="3" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" readingOrder="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="8" xfId="0" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="7" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="3" borderId="9" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1" readingOrder="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="10" xfId="0" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="11" xfId="0" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="12" xfId="0" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="13" xfId="0" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="14" xfId="0" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="6" fillId="0" borderId="7" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="3" fillId="5" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
@@ -1853,6 +1837,59 @@
     <xf numFmtId="164" fontId="10" fillId="6" borderId="3" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1" readingOrder="1"/>
     </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
+    <xf numFmtId="0" fontId="4" fillId="3" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" readingOrder="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="8" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="7" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="3" borderId="9" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1" readingOrder="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="10" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="11" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="12" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="13" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="14" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="7" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="7" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="7" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="7" borderId="17" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="164" fontId="3" fillId="7" borderId="3" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1" readingOrder="1"/>
+    </xf>
+    <xf numFmtId="164" fontId="3" fillId="7" borderId="17" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1" readingOrder="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="10" fillId="7" borderId="19" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="7" borderId="17" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="49" fontId="3" fillId="7" borderId="17" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="7" borderId="18" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="7" borderId="18" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="7" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normale" xfId="0" builtinId="0"/>
@@ -2342,10 +2379,10 @@
   <dimension ref="A1:T642"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="80" zoomScaleNormal="80" workbookViewId="0">
-      <pane xSplit="1" ySplit="9" topLeftCell="B10" activePane="bottomRight" state="frozen"/>
+      <pane xSplit="1" ySplit="9" topLeftCell="D34" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight" activeCell="B1" sqref="B1"/>
       <selection pane="bottomLeft" activeCell="A10" sqref="A10"/>
-      <selection pane="bottomRight" activeCell="I28" sqref="I28"/>
+      <selection pane="bottomRight" activeCell="K46" sqref="K46"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="14.42578125" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -2384,14 +2421,14 @@
       <c r="T1" s="15"/>
     </row>
     <row r="2" spans="1:20" ht="18.75" x14ac:dyDescent="0.25">
-      <c r="A2" s="52" t="s">
+      <c r="A2" s="63" t="s">
         <v>22</v>
       </c>
-      <c r="B2" s="53"/>
-      <c r="C2" s="54" t="s">
+      <c r="B2" s="64"/>
+      <c r="C2" s="65" t="s">
         <v>99</v>
       </c>
-      <c r="D2" s="53"/>
+      <c r="D2" s="64"/>
       <c r="F2" s="12"/>
       <c r="G2" s="12"/>
       <c r="H2" s="12"/>
@@ -2409,14 +2446,14 @@
       <c r="T2" s="15"/>
     </row>
     <row r="3" spans="1:20" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="A3" s="55" t="s">
+      <c r="A3" s="66" t="s">
         <v>23</v>
       </c>
-      <c r="B3" s="56"/>
-      <c r="C3" s="61" t="s">
+      <c r="B3" s="67"/>
+      <c r="C3" s="72" t="s">
         <v>102</v>
       </c>
-      <c r="D3" s="53"/>
+      <c r="D3" s="64"/>
       <c r="F3" s="12"/>
       <c r="G3" s="12"/>
       <c r="H3" s="12"/>
@@ -2434,12 +2471,12 @@
       <c r="T3" s="15"/>
     </row>
     <row r="4" spans="1:20" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="A4" s="57"/>
-      <c r="B4" s="58"/>
-      <c r="C4" s="61" t="s">
+      <c r="A4" s="68"/>
+      <c r="B4" s="69"/>
+      <c r="C4" s="72" t="s">
         <v>101</v>
       </c>
-      <c r="D4" s="53"/>
+      <c r="D4" s="64"/>
       <c r="E4" s="4"/>
       <c r="F4" s="12"/>
       <c r="G4" s="12"/>
@@ -2458,12 +2495,12 @@
       <c r="T4" s="15"/>
     </row>
     <row r="5" spans="1:20" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="A5" s="59"/>
-      <c r="B5" s="60"/>
-      <c r="C5" s="61" t="s">
+      <c r="A5" s="70"/>
+      <c r="B5" s="71"/>
+      <c r="C5" s="72" t="s">
         <v>100</v>
       </c>
-      <c r="D5" s="53"/>
+      <c r="D5" s="64"/>
       <c r="F5" s="12"/>
       <c r="G5" s="12"/>
       <c r="H5" s="12"/>
@@ -2481,8 +2518,8 @@
       <c r="T5" s="15"/>
     </row>
     <row r="6" spans="1:20" x14ac:dyDescent="0.25">
-      <c r="A6" s="50"/>
-      <c r="B6" s="51"/>
+      <c r="A6" s="61"/>
+      <c r="B6" s="62"/>
       <c r="C6" s="16"/>
       <c r="F6" s="12"/>
       <c r="G6" s="12"/>
@@ -2600,31 +2637,31 @@
       </c>
     </row>
     <row r="10" spans="1:20" ht="20.100000000000001" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A10" s="62">
+      <c r="A10" s="49">
         <v>1</v>
       </c>
-      <c r="B10" s="63" t="s">
+      <c r="B10" s="50" t="s">
         <v>44</v>
       </c>
-      <c r="C10" s="63" t="s">
+      <c r="C10" s="50" t="s">
         <v>45</v>
       </c>
-      <c r="D10" s="63" t="s">
+      <c r="D10" s="50" t="s">
         <v>46</v>
       </c>
-      <c r="E10" s="64" t="s">
+      <c r="E10" s="51" t="s">
         <v>47</v>
       </c>
-      <c r="F10" s="68">
+      <c r="F10" s="55">
         <v>45315</v>
       </c>
-      <c r="G10" s="70" t="s">
+      <c r="G10" s="57" t="s">
         <v>278</v>
       </c>
-      <c r="H10" s="69" t="s">
+      <c r="H10" s="56" t="s">
         <v>277</v>
       </c>
-      <c r="I10" s="69" t="s">
+      <c r="I10" s="56" t="s">
         <v>276</v>
       </c>
       <c r="J10" s="31" t="s">
@@ -2644,31 +2681,31 @@
       </c>
     </row>
     <row r="11" spans="1:20" ht="20.100000000000001" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A11" s="62">
+      <c r="A11" s="49">
         <v>2</v>
       </c>
-      <c r="B11" s="63" t="s">
+      <c r="B11" s="50" t="s">
         <v>44</v>
       </c>
-      <c r="C11" s="63" t="s">
+      <c r="C11" s="50" t="s">
         <v>45</v>
       </c>
-      <c r="D11" s="63" t="s">
+      <c r="D11" s="50" t="s">
         <v>49</v>
       </c>
-      <c r="E11" s="64" t="s">
+      <c r="E11" s="51" t="s">
         <v>50</v>
       </c>
-      <c r="F11" s="68">
+      <c r="F11" s="55">
         <v>45315</v>
       </c>
-      <c r="G11" s="70" t="s">
+      <c r="G11" s="57" t="s">
         <v>281</v>
       </c>
-      <c r="H11" s="69" t="s">
+      <c r="H11" s="56" t="s">
         <v>280</v>
       </c>
-      <c r="I11" s="69" t="s">
+      <c r="I11" s="56" t="s">
         <v>279</v>
       </c>
       <c r="J11" s="31" t="s">
@@ -2688,31 +2725,31 @@
       </c>
     </row>
     <row r="12" spans="1:20" ht="20.100000000000001" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A12" s="62">
+      <c r="A12" s="49">
         <v>3</v>
       </c>
-      <c r="B12" s="63" t="s">
+      <c r="B12" s="50" t="s">
         <v>44</v>
       </c>
-      <c r="C12" s="63" t="s">
+      <c r="C12" s="50" t="s">
         <v>45</v>
       </c>
-      <c r="D12" s="63" t="s">
+      <c r="D12" s="50" t="s">
         <v>51</v>
       </c>
-      <c r="E12" s="64" t="s">
+      <c r="E12" s="51" t="s">
         <v>52</v>
       </c>
-      <c r="F12" s="68">
+      <c r="F12" s="55">
         <v>45315</v>
       </c>
-      <c r="G12" s="70" t="s">
+      <c r="G12" s="57" t="s">
         <v>284</v>
       </c>
-      <c r="H12" s="69" t="s">
+      <c r="H12" s="56" t="s">
         <v>283</v>
       </c>
-      <c r="I12" s="69" t="s">
+      <c r="I12" s="56" t="s">
         <v>282</v>
       </c>
       <c r="J12" s="31" t="s">
@@ -2732,31 +2769,31 @@
       </c>
     </row>
     <row r="13" spans="1:20" ht="20.100000000000001" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A13" s="62">
+      <c r="A13" s="49">
         <v>4</v>
       </c>
-      <c r="B13" s="63" t="s">
+      <c r="B13" s="50" t="s">
         <v>44</v>
       </c>
-      <c r="C13" s="63" t="s">
+      <c r="C13" s="50" t="s">
         <v>45</v>
       </c>
-      <c r="D13" s="63" t="s">
+      <c r="D13" s="50" t="s">
         <v>53</v>
       </c>
-      <c r="E13" s="64" t="s">
+      <c r="E13" s="51" t="s">
         <v>54</v>
       </c>
-      <c r="F13" s="68">
+      <c r="F13" s="55">
         <v>45315</v>
       </c>
-      <c r="G13" s="70" t="s">
+      <c r="G13" s="57" t="s">
         <v>287</v>
       </c>
-      <c r="H13" s="69" t="s">
+      <c r="H13" s="56" t="s">
         <v>286</v>
       </c>
-      <c r="I13" s="69" t="s">
+      <c r="I13" s="56" t="s">
         <v>285</v>
       </c>
       <c r="J13" s="31" t="s">
@@ -2776,31 +2813,31 @@
       </c>
     </row>
     <row r="14" spans="1:20" ht="20.100000000000001" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A14" s="62">
+      <c r="A14" s="49">
         <v>5</v>
       </c>
-      <c r="B14" s="63" t="s">
+      <c r="B14" s="50" t="s">
         <v>44</v>
       </c>
-      <c r="C14" s="63" t="s">
+      <c r="C14" s="50" t="s">
         <v>45</v>
       </c>
-      <c r="D14" s="63" t="s">
+      <c r="D14" s="50" t="s">
         <v>55</v>
       </c>
-      <c r="E14" s="64" t="s">
+      <c r="E14" s="51" t="s">
         <v>56</v>
       </c>
-      <c r="F14" s="68">
+      <c r="F14" s="55">
         <v>45315</v>
       </c>
-      <c r="G14" s="70" t="s">
+      <c r="G14" s="57" t="s">
         <v>290</v>
       </c>
-      <c r="H14" s="69" t="s">
+      <c r="H14" s="56" t="s">
         <v>289</v>
       </c>
-      <c r="I14" s="69" t="s">
+      <c r="I14" s="56" t="s">
         <v>288</v>
       </c>
       <c r="J14" s="31" t="s">
@@ -2820,31 +2857,31 @@
       </c>
     </row>
     <row r="15" spans="1:20" ht="20.100000000000001" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A15" s="62">
+      <c r="A15" s="49">
         <v>28</v>
       </c>
-      <c r="B15" s="63" t="s">
+      <c r="B15" s="50" t="s">
         <v>44</v>
       </c>
-      <c r="C15" s="63" t="s">
+      <c r="C15" s="50" t="s">
         <v>45</v>
       </c>
-      <c r="D15" s="63" t="s">
+      <c r="D15" s="50" t="s">
         <v>58</v>
       </c>
-      <c r="E15" s="64" t="s">
+      <c r="E15" s="51" t="s">
         <v>59</v>
       </c>
-      <c r="F15" s="68">
+      <c r="F15" s="55">
         <v>45315</v>
       </c>
-      <c r="G15" s="70" t="s">
+      <c r="G15" s="57" t="s">
         <v>292</v>
       </c>
-      <c r="H15" s="69" t="s">
+      <c r="H15" s="56" t="s">
         <v>291</v>
       </c>
-      <c r="I15" s="69" t="s">
+      <c r="I15" s="56" t="s">
         <v>103</v>
       </c>
       <c r="J15" s="31" t="s">
@@ -2874,28 +2911,28 @@
       </c>
     </row>
     <row r="16" spans="1:20" ht="20.100000000000001" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A16" s="62">
+      <c r="A16" s="49">
         <v>36</v>
       </c>
-      <c r="B16" s="63" t="s">
+      <c r="B16" s="50" t="s">
         <v>44</v>
       </c>
-      <c r="C16" s="63" t="s">
+      <c r="C16" s="50" t="s">
         <v>45</v>
       </c>
-      <c r="D16" s="63" t="s">
+      <c r="D16" s="50" t="s">
         <v>62</v>
       </c>
-      <c r="E16" s="64" t="s">
+      <c r="E16" s="51" t="s">
         <v>63</v>
       </c>
-      <c r="F16" s="68">
+      <c r="F16" s="55">
         <v>45315</v>
       </c>
-      <c r="G16" s="70" t="s">
+      <c r="G16" s="57" t="s">
         <v>294</v>
       </c>
-      <c r="H16" s="70" t="s">
+      <c r="H16" s="57" t="s">
         <v>293</v>
       </c>
       <c r="I16" s="30" t="s">
@@ -3354,31 +3391,31 @@
       </c>
     </row>
     <row r="28" spans="1:20" ht="20.100000000000001" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A28" s="65">
+      <c r="A28" s="52">
         <v>62</v>
       </c>
-      <c r="B28" s="66" t="s">
+      <c r="B28" s="53" t="s">
         <v>44</v>
       </c>
-      <c r="C28" s="66" t="s">
+      <c r="C28" s="53" t="s">
         <v>45</v>
       </c>
-      <c r="D28" s="66" t="s">
+      <c r="D28" s="53" t="s">
         <v>120</v>
       </c>
-      <c r="E28" s="67" t="s">
+      <c r="E28" s="54" t="s">
         <v>121</v>
       </c>
-      <c r="F28" s="73">
+      <c r="F28" s="60">
         <v>45315</v>
       </c>
-      <c r="G28" s="72" t="s">
+      <c r="G28" s="59" t="s">
         <v>297</v>
       </c>
-      <c r="H28" s="71" t="s">
+      <c r="H28" s="58" t="s">
         <v>295</v>
       </c>
-      <c r="I28" s="71" t="s">
+      <c r="I28" s="58" t="s">
         <v>296</v>
       </c>
       <c r="J28" s="31" t="s">
@@ -4085,7 +4122,7 @@
       <c r="G45" s="30"/>
       <c r="H45" s="30"/>
       <c r="I45" s="30"/>
-      <c r="J45" s="48" t="s">
+      <c r="J45" s="47" t="s">
         <v>98</v>
       </c>
       <c r="K45" s="24" t="s">
@@ -4103,41 +4140,41 @@
         <v>60</v>
       </c>
     </row>
-    <row r="46" spans="1:20" s="46" customFormat="1" ht="20.100000000000001" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A46" s="25">
+    <row r="46" spans="1:20" s="83" customFormat="1" ht="20.100000000000001" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A46" s="73">
         <v>84</v>
       </c>
-      <c r="B46" s="26" t="s">
+      <c r="B46" s="74" t="s">
         <v>44</v>
       </c>
-      <c r="C46" s="26" t="s">
+      <c r="C46" s="74" t="s">
         <v>57</v>
       </c>
-      <c r="D46" s="26" t="s">
+      <c r="D46" s="74" t="s">
         <v>152</v>
       </c>
-      <c r="E46" s="27" t="s">
+      <c r="E46" s="75" t="s">
         <v>153</v>
       </c>
-      <c r="F46" s="28"/>
-      <c r="G46" s="30"/>
-      <c r="H46" s="30"/>
-      <c r="I46" s="30"/>
-      <c r="J46" s="47" t="s">
+      <c r="F46" s="76"/>
+      <c r="G46" s="77"/>
+      <c r="H46" s="77"/>
+      <c r="I46" s="77"/>
+      <c r="J46" s="78" t="s">
         <v>98</v>
       </c>
-      <c r="K46" s="31" t="s">
-        <v>237</v>
-      </c>
-      <c r="L46" s="31"/>
-      <c r="M46" s="31"/>
-      <c r="N46" s="31"/>
-      <c r="O46" s="31"/>
-      <c r="P46" s="31"/>
-      <c r="Q46" s="31"/>
-      <c r="R46" s="32"/>
-      <c r="S46" s="33"/>
-      <c r="T46" s="34" t="s">
+      <c r="K46" s="79" t="s">
+        <v>298</v>
+      </c>
+      <c r="L46" s="79"/>
+      <c r="M46" s="79"/>
+      <c r="N46" s="79"/>
+      <c r="O46" s="79"/>
+      <c r="P46" s="79"/>
+      <c r="Q46" s="79"/>
+      <c r="R46" s="80"/>
+      <c r="S46" s="81"/>
+      <c r="T46" s="82" t="s">
         <v>60</v>
       </c>
     </row>
@@ -4652,7 +4689,7 @@
       </c>
     </row>
     <row r="59" spans="1:20" s="46" customFormat="1" ht="20.100000000000001" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A59" s="49">
+      <c r="A59" s="48">
         <v>147</v>
       </c>
       <c r="B59" s="26" t="s">
@@ -4696,7 +4733,7 @@
       </c>
     </row>
     <row r="60" spans="1:20" s="46" customFormat="1" ht="20.100000000000001" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A60" s="49">
+      <c r="A60" s="48">
         <v>148</v>
       </c>
       <c r="B60" s="26" t="s">
@@ -4734,7 +4771,7 @@
       </c>
     </row>
     <row r="61" spans="1:20" s="46" customFormat="1" ht="20.100000000000001" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A61" s="49">
+      <c r="A61" s="48">
         <v>149</v>
       </c>
       <c r="B61" s="26" t="s">
@@ -4772,7 +4809,7 @@
       </c>
     </row>
     <row r="62" spans="1:20" s="46" customFormat="1" ht="20.100000000000001" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A62" s="49">
+      <c r="A62" s="48">
         <v>150</v>
       </c>
       <c r="B62" s="26" t="s">

</xml_diff>